<commit_message>
updated model comparison results on the v9 full feature set
</commit_message>
<xml_diff>
--- a/data/processed/model_metrics_comparison_with_raw.xlsx
+++ b/data/processed/model_metrics_comparison_with_raw.xlsx
@@ -483,14 +483,14 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.8558474046278924</v>
+        <v>0.8560677734590778</v>
       </c>
       <c r="E2" t="n">
-        <v>0.007573147856817064</v>
+        <v>0.01000132555673383</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[0.8695652173913043, 0.8406349206349206, 0.8564102564102565, 0.8372598162071847, 0.8616021659499921, 0.8524691358024691, 0.8552845528455284, 0.8822222222222222, 0.8581780538302277, 0.8552845528455284]</t>
+          <t>[0.8557252905078991, 0.8524691358024691, 0.8564102564102565, 0.8547101449275362, 0.8819047619047619, 0.8708259061200238, 0.8419622425629292, 0.8666666666666667, 0.8594202898550726, 0.8552845528455284]</t>
         </is>
       </c>
     </row>
@@ -514,11 +514,11 @@
         <v>0.8572463768115942</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02101449275362322</v>
+        <v>0.01884057971014497</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[0.8666666666666667, 0.8478260869565217, 0.8478260869565217, 0.8444444444444444, 0.8695652173913043, 0.8478260869565217, 0.8666666666666667, 0.8695652173913043, 0.8695652173913043, 0.8478260869565217]</t>
+          <t>[0.8478260869565217, 0.8478260869565217, 0.8666666666666667, 0.8478260869565217, 0.8695652173913043, 0.8695652173913043, 0.8478260869565217, 0.8478260869565217, 0.8666666666666667, 0.8666666666666667]</t>
         </is>
       </c>
     </row>
@@ -539,14 +539,14 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.8581081081081081</v>
+        <v>0.8644252805437016</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01689189189189177</v>
+        <v>0.03922672672672678</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[0.8648648648648648, 0.8344594594594595, 0.8682432432432432, 0.847972972972973, 0.8648648648648648, 0.847972972972973, 0.9324324324324325, 0.8614864864864865, 0.8547297297297297, 0.8355263157894737]</t>
+          <t>[0.8412162162162162, 0.8828828828828829, 0.8798798798798799, 0.8344594594594594, 0.902027027027027, 0.8768768768768769, 0.9009009009009009, 0.8479729729729729, 0.8258258258258258, 0.8519736842105263]</t>
         </is>
       </c>
     </row>
@@ -567,14 +567,14 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8458025066720719</v>
+        <v>0.8525322675819526</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01354984112811786</v>
+        <v>0.01046519565194992</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[0.843741765480896, 0.8355731225296441, 0.8158942506768594, 0.8402962962962963, 0.863129290617849, 0.8479541588324827, 0.8478632478632478, 0.8750489620054837, 0.851086956521739, 0.8331569366241903]</t>
+          <t>[0.8418478260869564, 0.8479541588324827, 0.8588972431077694, 0.8507883765399203, 0.8722222222222222, 0.8542761586239848, 0.8443648763853367, 0.8567129557067178, 0.8588972431077694, 0.8478632478632478]</t>
         </is>
       </c>
     </row>
@@ -595,14 +595,14 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.8674749163879598</v>
+        <v>0.8316261668664415</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02264061421670105</v>
+        <v>0.02138121428234496</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[0.8386749482401656, 0.8674749163879598, 0.8479096989966556, 0.8809523809523808, 0.8260869565217391, 0.8764367816091954, 0.8674749163879598, 0.8674749163879598, 0.8458994708994709, 0.8695652173913043]</t>
+          <t>[0.8260869565217391, 0.827273497754047, 0.7995951417004049, 0.8260869565217391, 0.8490612648221345, 0.8056653491436101, 0.8485060690943044, 0.835978835978836, 0.8443544759334234, 0.8490612648221345]</t>
         </is>
       </c>
     </row>
@@ -623,14 +623,14 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.8478260869565217</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01666666666666683</v>
+        <v>0.02125603864734293</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[0.8260869565217391, 0.8478260869565217, 0.8478260869565217, 0.8666666666666667, 0.8260869565217391, 0.8666666666666667, 0.8478260869565217, 0.8478260869565217, 0.8444444444444444, 0.8695652173913043]</t>
+          <t>[0.8260869565217391, 0.8260869565217391, 0.8, 0.8222222222222222, 0.8478260869565217, 0.8043478260869565, 0.8444444444444444, 0.8260869565217391, 0.8444444444444444, 0.8478260869565217]</t>
         </is>
       </c>
     </row>
@@ -651,14 +651,14 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.9210476190476191</v>
+        <v>0.9161428571428571</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01619047619047631</v>
+        <v>0.01049999999999995</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[0.9161904761904761, 0.924, 0.9123809523809523, 0.908, 0.9180952380952381, 0.9314285714285714, 0.936, 0.9295238095238095, 0.9295238095238095, 0.9009523809523811]</t>
+          <t>[0.8952380952380952, 0.9142857142857143, 0.8933333333333333, 0.918, 0.9123809523809523, 0.9257142857142857, 0.9371428571428572, 0.9180952380952381, 0.906, 0.9180952380952381]</t>
         </is>
       </c>
     </row>
@@ -679,14 +679,14 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.8474663377531092</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01458355905656805</v>
+        <v>0.02107424839292804</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[0.8264163372859025, 0.8474663377531092, 0.8474622086374317, 0.8669301712779972, 0.8260869565217391, 0.8641975308641976, 0.8474663377531092, 0.8474663377531092, 0.8447541618273327, 0.8695652173913043]</t>
+          <t>[0.8260869565217391, 0.8250836120401338, 0.7993966817496228, 0.8216952129995607, 0.8480427560306225, 0.8046264006108004, 0.8425406538614084, 0.8260869565217391, 0.8439751969163732, 0.8480427560306225]</t>
         </is>
       </c>
     </row>
@@ -707,14 +707,14 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.8449488491048593</v>
+        <v>0.8470737835267886</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02972631987577645</v>
+        <v>0.02482766508758738</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[0.8375388198757764, 0.8449488491048593, 0.8716542629586108, 0.8895993179880648, 0.8449488491048593, 0.8666666666666667, 0.8695652173913043, 0.843840579710145, 0.8260869565217391, 0.8337941628264208]</t>
+          <t>[0.8449488491048593, 0.8491987179487179, 0.8764976958525345, 0.8695652173913043, 0.8666666666666667, 0.8222222222222222, 0.8180778032036613, 0.8409982174688057, 0.8363721365123888, 0.8494252873563217]</t>
         </is>
       </c>
     </row>
@@ -735,14 +735,14 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.8478260869565217</v>
+        <v>0.846135265700483</v>
       </c>
       <c r="E11" t="n">
-        <v>0.03345410628019319</v>
+        <v>0.03586956521739137</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[0.8260869565217391, 0.8478260869565217, 0.8695652173913043, 0.8888888888888888, 0.8478260869565217, 0.8478260869565217, 0.8695652173913043, 0.8444444444444444, 0.8260869565217391, 0.8222222222222222]</t>
+          <t>[0.8478260869565217, 0.8478260869565217, 0.8666666666666667, 0.8695652173913043, 0.8666666666666667, 0.8222222222222222, 0.8260869565217391, 0.8444444444444444, 0.8260869565217391, 0.8260869565217391]</t>
         </is>
       </c>
     </row>
@@ -763,14 +763,14 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.8992498514557339</v>
+        <v>0.9027777777777777</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01948786507610034</v>
+        <v>0.01743395493395494</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[0.875, 0.8951048951048951, 0.9117647058823529, 0.9393939393939394, 0.9141414141414141, 0.898989898989899, 0.8995098039215687, 0.8838383838383839, 0.9090909090909092, 0.8904428904428905]</t>
+          <t>[0.8857808857808858, 0.9065656565656566, 0.9166666666666666, 0.9090909090909091, 0.9166666666666667, 0.8585858585858586, 0.8904428904428904, 0.8989898989898989, 0.8927738927738929, 0.9065656565656565]</t>
         </is>
       </c>
     </row>
@@ -791,14 +791,14 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.8459182349123945</v>
+        <v>0.8440709495998269</v>
       </c>
       <c r="E13" t="n">
-        <v>0.03273118559661436</v>
+        <v>0.03200899824812875</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[0.8301408736191344, 0.8459182349123945, 0.8695652173913043, 0.8899415963659961, 0.8459182349123945, 0.8538615409376221, 0.8695652173913043, 0.8412098298676749, 0.8260869565217391, 0.8262820512820512]</t>
+          <t>[0.8459182349123945, 0.8463589743589742, 0.8697115384615384, 0.8695652173913043, 0.8666666666666667, 0.8222222222222222, 0.8135265700483091, 0.8422236642872594, 0.8295807453416149, 0.8295807453416149]</t>
         </is>
       </c>
     </row>
@@ -819,14 +819,14 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.7648341694537346</v>
+        <v>0.7735685780298256</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02877365689865674</v>
+        <v>0.03274801325013987</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[0.7759387351778656, 0.7247234247234247, 0.766499442586399, 0.7735228539576365, 0.7567758328627895, 0.7431561996779389, 0.7794732441471572, 0.782608695652174, 0.7631688963210703, 0.7391304347826086]</t>
+          <t>[0.8185185185185185, 0.7610671936758893, 0.7822222222222223, 0.7318840579710144, 0.7755555555555556, 0.74515595463138, 0.7850574712643679, 0.7808604439039222, 0.742889341282536, 0.7715816005040957]</t>
         </is>
       </c>
     </row>
@@ -847,14 +847,14 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.7608695652173914</v>
+        <v>0.7582125603864734</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01763285024154593</v>
+        <v>0.03864734299516914</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[0.7608695652173914, 0.7333333333333333, 0.7608695652173914, 0.7555555555555555, 0.7608695652173914, 0.7391304347826086, 0.782608695652174, 0.7777777777777778, 0.7608695652173914, 0.7391304347826086]</t>
+          <t>[0.8043478260869565, 0.7391304347826086, 0.782608695652174, 0.7391304347826086, 0.7777777777777778, 0.7391304347826086, 0.7777777777777778, 0.7555555555555555, 0.7391304347826086, 0.7608695652173914]</t>
         </is>
       </c>
     </row>
@@ -875,14 +875,14 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.9080939986317561</v>
+        <v>0.893482037899187</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0130474516818575</v>
+        <v>0.03170376883763604</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[0.8848727550100548, 0.9140258440258442, 0.918808879907278, 0.8993629993629993, 0.9139276055752028, 0.899291212220274, 0.9377104543344952, 0.9065101465101465, 0.9096778507533657, 0.9057263328363072]</t>
+          <t>[0.901209391209391, 0.8736409136409135, 0.8778294550605763, 0.8889879100876543, 0.9166066066066065, 0.8795049595049593, 0.9214532714532715, 0.8783929383929384, 0.9134298196083093, 0.8979761657107196]</t>
         </is>
       </c>
     </row>
@@ -903,14 +903,14 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.7557957283654577</v>
+        <v>0.7593540416909981</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01982132149718652</v>
+        <v>0.03236134886484721</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[0.764084123351858, 0.7251220750810577, 0.7595907928388747, 0.7560541310541311, 0.7555373256767843, 0.7379359770664119, 0.7803069053708439, 0.782608695652174, 0.7551665725578769, 0.7391304347826086]</t>
+          <t>[0.8022448565926826, 0.7452492289324446, 0.7790281329923272, 0.7329192546583849, 0.773135124833238, 0.7385798522307475, 0.7710288065843621, 0.7543447293447293, 0.731296851574213, 0.7643633540372669]</t>
         </is>
       </c>
     </row>
@@ -1379,14 +1379,14 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.8299957927835167</v>
+        <v>0.8256606990622337</v>
       </c>
       <c r="E34" t="n">
-        <v>0.03879872200075773</v>
+        <v>0.04367779845602437</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[0.8061443932411674, 0.7992592592592593, 0.8256606990622337, 0.8406349206349206, 0.8528846153846155, 0.8256606990622337, 0.8612794612794613, 0.8708259061200238, 0.7992592592592593, 0.8343308865047995]</t>
+          <t>[0.8061443932411674, 0.7992592592592593, 0.8256606990622337, 0.8406349206349206, 0.8528846153846155, 0.8256606990622337, 0.8612794612794613, 0.8708259061200238, 0.7992592592592593, 0.8061443932411674]</t>
         </is>
       </c>
     </row>
@@ -1410,11 +1410,11 @@
         <v>0.7826086956521739</v>
       </c>
       <c r="E35" t="n">
-        <v>0.02173913043478259</v>
+        <v>0.01992753623188404</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[0.782608695652174, 0.7555555555555555, 0.782608695652174, 0.8043478260869565, 0.8222222222222222, 0.782608695652174, 0.8222222222222222, 0.782608695652174, 0.7608695652173914, 0.8043478260869565]</t>
+          <t>[0.782608695652174, 0.7391304347826086, 0.782608695652174, 0.8043478260869565, 0.8222222222222222, 0.7777777777777778, 0.8222222222222222, 0.782608695652174, 0.7608695652173914, 0.782608695652174]</t>
         </is>
       </c>
     </row>
@@ -1438,11 +1438,11 @@
         <v>0.8116998577524894</v>
       </c>
       <c r="E36" t="n">
-        <v>0.05894381223328604</v>
+        <v>0.05641002844950216</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>[0.8141891891891893, 0.7631578947368421, 0.8040540540540541, 0.7736486486486486, 0.8344594594594594, 0.8421052631578948, 0.8817567567567568, 0.888157894736842, 0.7263513513513513, 0.8092105263157895]</t>
+          <t>[0.8141891891891893, 0.7631578947368421, 0.8040540540540541, 0.7770270270270271, 0.8344594594594594, 0.8421052631578948, 0.8783783783783784, 0.8848684210526316, 0.7297297297297297, 0.8092105263157895]</t>
         </is>
       </c>
     </row>
@@ -1463,14 +1463,14 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.80218101733447</v>
+        <v>0.7983091787439613</v>
       </c>
       <c r="E37" t="n">
-        <v>0.02681478423844741</v>
+        <v>0.02602477535480974</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0.7885940146809712, 0.7696894819207644, 0.7983091787439613, 0.8185255198487712, 0.8296296296296297, 0.7983091787439613, 0.8349206349206348, 0.8060528559249787, 0.7781978575929426, 0.8157738001943514]</t>
+          <t>[0.7885940146809712, 0.7672634271099745, 0.7983091787439613, 0.8185255198487712, 0.8296296296296297, 0.7983091787439613, 0.8349206349206348, 0.8060528559249787, 0.7781978575929426, 0.7917482700091397]</t>
         </is>
       </c>
     </row>
@@ -1491,14 +1491,14 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.7329218106995885</v>
+        <v>0.7429111531190926</v>
       </c>
       <c r="E38" t="n">
-        <v>0.03881536719065326</v>
+        <v>0.02231425778707286</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[0.7325102880658436, 0.7548358074673864, 0.7604515050167224, 0.7188735177865612, 0.7188735177865612, 0.7333333333333333, 0.7165013984235952, 0.7882529323573506, 0.7620137299771167, 0.7243083003952568]</t>
+          <t>[0.7429111531190926, 0.7332775919732442, 0.7622694334650856, 0.7680335968379446, 0.7503933747412009, 0.7165013984235952, 0.7165013984235952, 0.7426580827233442, 0.7604515050167224, 0.7429111531190926]</t>
         </is>
       </c>
     </row>
@@ -1519,14 +1519,14 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.7253623188405797</v>
+        <v>0.7391304347826086</v>
       </c>
       <c r="E39" t="n">
-        <v>0.03816425120772948</v>
+        <v>0.03405797101449271</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[0.717391304347826, 0.7555555555555555, 0.7608695652173914, 0.7111111111111111, 0.717391304347826, 0.7333333333333333, 0.7111111111111111, 0.7555555555555555, 0.7555555555555555, 0.717391304347826]</t>
+          <t>[0.7391304347826086, 0.717391304347826, 0.7608695652173914, 0.7608695652173914, 0.7391304347826086, 0.6956521739130435, 0.6956521739130435, 0.7333333333333333, 0.7608695652173914, 0.7391304347826086]</t>
         </is>
       </c>
     </row>
@@ -1547,14 +1547,14 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.7911904761904762</v>
+        <v>0.7774761904761904</v>
       </c>
       <c r="E40" t="n">
-        <v>0.03335714285714286</v>
+        <v>0.02957142857142858</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[0.79, 0.7523809523809524, 0.7639999999999999, 0.7679999999999999, 0.8228571428571428, 0.8038095238095239, 0.77, 0.7923809523809524, 0.8171428571428572, 0.796]</t>
+          <t>[0.774, 0.76, 0.7714285714285715, 0.806, 0.8495238095238095, 0.768, 0.780952380952381, 0.7885714285714286, 0.8285714285714285, 0.774]</t>
         </is>
       </c>
     </row>
@@ -1575,14 +1575,14 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.7255627505396238</v>
+        <v>0.7393774703557312</v>
       </c>
       <c r="E41" t="n">
-        <v>0.03758874009275481</v>
+        <v>0.03424449393685092</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[0.7177921677459144, 0.7548181665828725, 0.7602977564302497, 0.7091099015888724, 0.7167231986843458, 0.7333333333333333, 0.7116863005364747, 0.7538622244213535, 0.7548181665828725, 0.7177921677459144]</t>
+          <t>[0.7396245059288536, 0.7177936897711562, 0.7612100451909782, 0.761208757323466, 0.7391304347826089, 0.6956521739130435, 0.6939229249011858, 0.7301587301587302, 0.7602977564302497, 0.7396245059288536]</t>
         </is>
       </c>
     </row>
@@ -1603,14 +1603,14 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.7678380977578437</v>
+        <v>0.7672043219461698</v>
       </c>
       <c r="E42" t="n">
-        <v>0.01098818150448577</v>
+        <v>0.01170884817570195</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[0.7676190476190476, 0.7943899018232818, 0.7777777777777778, 0.7562111801242236, 0.7655172413793104, 0.7680571478966398, 0.766789596273292, 0.7777777777777778, 0.766789596273292, 0.7807065217391305]</t>
+          <t>[0.7676190476190476, 0.7943899018232818, 0.7655172413793104, 0.7680571478966398, 0.766789596273292, 0.8093944099378882, 0.7540760869565217, 0.7547148503670243, 0.766789596273292, 0.7807065217391305]</t>
         </is>
       </c>
     </row>
@@ -1631,14 +1631,14 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7608695652173914</v>
       </c>
       <c r="E43" t="n">
-        <v>0.01763285024154593</v>
+        <v>0.02173913043478271</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[0.7391304347826086, 0.782608695652174, 0.7555555555555555, 0.7391304347826086, 0.7333333333333333, 0.7555555555555555, 0.7608695652173914, 0.7555555555555555, 0.7608695652173914, 0.7608695652173914]</t>
+          <t>[0.7608695652173914, 0.782608695652174, 0.7333333333333333, 0.7391304347826086, 0.7333333333333333, 0.782608695652174, 0.7391304347826086, 0.7608695652173914, 0.7608695652173914, 0.7608695652173914]</t>
         </is>
       </c>
     </row>
@@ -1659,14 +1659,14 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.7727272727272727</v>
+        <v>0.7806915306915307</v>
       </c>
       <c r="E44" t="n">
-        <v>0.03117715617715622</v>
+        <v>0.03904000411353359</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[0.7878787878787878, 0.7297979797979798, 0.7929292929292929, 0.8111888111888111, 0.7598039215686274, 0.803030303030303, 0.7622377622377623, 0.7622377622377622, 0.7832167832167832, 0.7599067599067599]</t>
+          <t>[0.8018648018648019, 0.7323232323232323, 0.7828282828282829, 0.8158508158508159, 0.7622377622377622, 0.8259803921568627, 0.7622549019607844, 0.7785547785547785, 0.7995337995337995, 0.7575757575757577]</t>
         </is>
       </c>
     </row>
@@ -1687,14 +1687,14 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.76331569664903</v>
+        <v>0.7574039067422811</v>
       </c>
       <c r="E45" t="n">
-        <v>0.01535184985395377</v>
+        <v>0.01837430028536091</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[0.7481065918653576, 0.7869759316770187, 0.76331569664903, 0.7391304347826086, 0.743778801843318, 0.7481065918653576, 0.7634584417193113, 0.76331569664903, 0.7634584417193113, 0.7675447990290568]</t>
+          <t>[0.7574039067422811, 0.7869759316770187, 0.743778801843318, 0.7481065918653576, 0.7482758620689655, 0.7900888265544647, 0.7452113104287017, 0.7574039067422811, 0.7634584417193113, 0.7675447990290568]</t>
         </is>
       </c>
     </row>
@@ -1718,11 +1718,11 @@
         <v>0.6577040427154843</v>
       </c>
       <c r="E46" t="n">
-        <v>0.02138464573819265</v>
+        <v>0.01984916454797991</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[0.6545893719806763, 0.6521739130434783, 0.6721343873517787, 0.6730887825624667, 0.6608187134502924, 0.6336899010812054, 0.6616267942583732, 0.6467724867724868, 0.6419753086419753, 0.6832298136645962]</t>
+          <t>[0.6545893719806763, 0.6521739130434783, 0.6830947880097219, 0.6730887825624667, 0.6608187134502924, 0.6362876254180602, 0.6650515176830966, 0.6467724867724868, 0.6419753086419753, 0.668945504623254]</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[0.6086956521739131, 0.6304347826086957, 0.6304347826086957, 0.6304347826086957, 0.6304347826086957, 0.6521739130434783, 0.6222222222222222, 0.6222222222222222, 0.5869565217391305, 0.5869565217391305]</t>
+          <t>[0.6086956521739131, 0.6304347826086957, 0.6304347826086957, 0.6521739130434783, 0.6304347826086957, 0.6521739130434783, 0.6222222222222222, 0.6222222222222222, 0.5869565217391305, 0.5869565217391305]</t>
         </is>
       </c>
     </row>
@@ -1771,14 +1771,14 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.7996411060827537</v>
+        <v>0.8020283871199203</v>
       </c>
       <c r="E48" t="n">
-        <v>0.01452549736874675</v>
+        <v>0.01007171162138176</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[0.7987780716613669, 0.7698007098007098, 0.7732002932231765, 0.807998907998908, 0.8173382473382473, 0.8079041477210813, 0.8005041405041405, 0.8314805714805715, 0.7919592319592319, 0.7979211863651223]</t>
+          <t>[0.7982258016582959, 0.7792901992901994, 0.7802584524552488, 0.8039020839020838, 0.8219065450186732, 0.8098044153031365, 0.8026535626535627, 0.8365256165256167, 0.7983510783510783, 0.801403211586278]</t>
         </is>
       </c>
     </row>
@@ -1799,14 +1799,14 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.6306311604308488</v>
+        <v>0.630914395406954</v>
       </c>
       <c r="E49" t="n">
-        <v>0.02356082778253665</v>
+        <v>0.0217967994715651</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[0.6073356337704164, 0.6308824992538057, 0.6400488965243822, 0.6382974202048536, 0.6309462915601023, 0.6390746934225195, 0.6303798216078917, 0.6295883397332672, 0.5853807789982559, 0.5918194748779456]</t>
+          <t>[0.6118012422360248, 0.6308824992538057, 0.6414618777567738, 0.6489687848383501, 0.6309462915601023, 0.6401333108494235, 0.6317793317793318, 0.6295883397332672, 0.5853807789982559, 0.5836317135549872]</t>
         </is>
       </c>
     </row>
@@ -1827,14 +1827,14 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.8097826086956522</v>
+        <v>0.8044413277232352</v>
       </c>
       <c r="E50" t="n">
-        <v>0.02084307308711242</v>
+        <v>0.02943094451726158</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[0.8342391304347826, 0.7947125338429687, 0.8524691358024691, 0.8047685834502104, 0.8041140719962598, 0.8260869565217391, 0.7815217391304349, 0.8097826086956522, 0.8097826086956522, 0.8222222222222222]</t>
+          <t>[0.8342391304347826, 0.7947125338429687, 0.8720355731225296, 0.8047685834502104, 0.8041140719962598, 0.8304812834224597, 0.7815217391304349, 0.8097826086956522, 0.7993650793650795, 0.7902255639097746]</t>
         </is>
       </c>
     </row>
@@ -1855,14 +1855,14 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.8241545893719806</v>
+        <v>0.8043478260869565</v>
       </c>
       <c r="E51" t="n">
-        <v>0.04166666666666663</v>
+        <v>0.02512077294685988</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[0.8260869565217391, 0.8043478260869565, 0.8444444444444444, 0.7608695652173914, 0.7777777777777778, 0.8260869565217391, 0.7555555555555555, 0.8260869565217391, 0.8260869565217391, 0.8222222222222222]</t>
+          <t>[0.8222222222222222, 0.8043478260869565, 0.8478260869565217, 0.7608695652173914, 0.8, 0.8260869565217391, 0.7608695652173914, 0.8260869565217391, 0.8043478260869565, 0.8]</t>
         </is>
       </c>
     </row>
@@ -1883,14 +1883,14 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.6504934210526316</v>
+        <v>0.6500266714082503</v>
       </c>
       <c r="E52" t="n">
-        <v>0.05962171052631571</v>
+        <v>0.046875</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>[0.6940789473684211, 0.6348684210526316, 0.6315789473684211, 0.7162162162162162, 0.6381578947368421, 0.6957236842105263, 0.618421052631579, 0.6529605263157895, 0.6480263157894737, 0.6976351351351351]</t>
+          <t>[0.7072368421052632, 0.6348684210526316, 0.6315789473684211, 0.7162162162162162, 0.6381578947368421, 0.6973684210526315, 0.6520270270270271, 0.6480263157894737, 0.6480263157894737, 0.6578947368421052]</t>
         </is>
       </c>
     </row>
@@ -1911,14 +1911,14 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.8109383906485356</v>
+        <v>0.7968816111424808</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0435989789907345</v>
+        <v>0.02330414298530237</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[0.8333986160073116, 0.7990965556182948, 0.8059825306202117, 0.766308610400682, 0.766308610400682, 0.8260869565217391, 0.7696894819207644, 0.8158942506768594, 0.8158942506768594, 0.8222222222222222]</t>
+          <t>[0.8296296296296297, 0.7990965556182948, 0.8059825306202117, 0.766308610400682, 0.7946666666666667, 0.8260869565217391, 0.7696894819207644, 0.8158942506768594, 0.7885940146809712, 0.7946666666666667]</t>
         </is>
       </c>
     </row>
@@ -1939,14 +1939,14 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.8260869565217391</v>
+        <v>0.8079697476436607</v>
       </c>
       <c r="E54" t="n">
-        <v>0.03039795506950527</v>
+        <v>0.03052062583545578</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>[0.804180602006689, 0.8260869565217391, 0.7777777777777778, 0.8443544759334234, 0.8260869565217391, 0.8386749482401656, 0.7548358074673864, 0.8117588932806324, 0.8393719806763286, 0.8298676748582231]</t>
+          <t>[0.822742474916388, 0.804180602006689, 0.7928743961352657, 0.7988779803646564, 0.8554841897233202, 0.7945341614906832, 0.783117213323163, 0.8117588932806324, 0.827273497754047, 0.8298676748582231]</t>
         </is>
       </c>
     </row>
@@ -1967,14 +1967,14 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.8241545893719806</v>
+        <v>0.8043478260869565</v>
       </c>
       <c r="E55" t="n">
         <v>0.02173913043478259</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[0.8043478260869565, 0.8260869565217391, 0.7608695652173914, 0.8444444444444444, 0.8260869565217391, 0.8260869565217391, 0.7555555555555555, 0.8043478260869565, 0.8222222222222222, 0.8260869565217391]</t>
+          <t>[0.8043478260869565, 0.8043478260869565, 0.7777777777777778, 0.782608695652174, 0.8478260869565217, 0.782608695652174, 0.782608695652174, 0.8043478260869565, 0.8043478260869565, 0.8260869565217391]</t>
         </is>
       </c>
     </row>
@@ -1995,14 +1995,14 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.8034523809523809</v>
+        <v>0.8376190476190476</v>
       </c>
       <c r="E56" t="n">
-        <v>0.04238095238095219</v>
+        <v>0.009797619047619111</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[0.7942857142857143, 0.7819047619047621, 0.72, 0.8095238095238095, 0.8342857142857143, 0.8019047619047619, 0.7571428571428571, 0.8049999999999999, 0.8333333333333334, 0.8447619047619048]</t>
+          <t>[0.8352380952380952, 0.8580952380952381, 0.8160000000000001, 0.8447619047619047, 0.8523809523809524, 0.8057142857142856, 0.84, 0.8342857142857143, 0.843, 0.8352380952380952]</t>
         </is>
       </c>
     </row>
@@ -2023,14 +2023,14 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.8235248097948327</v>
+        <v>0.803138893476945</v>
       </c>
       <c r="E57" t="n">
-        <v>0.02202063289610434</v>
+        <v>0.02211429970738477</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[0.8038799825338406, 0.8260869565217391, 0.7584862054022822, 0.8439751969163732, 0.8260869565217391, 0.8260869565217391, 0.7548181665828725, 0.8046253469010175, 0.8209626630679262, 0.8264163372859025]</t>
+          <t>[0.8038852913968547, 0.8038799825338406, 0.7777777777777778, 0.7813545150501673, 0.8474663377531092, 0.7830204216073781, 0.7813545150501673, 0.8038852913968547, 0.8023978044200493, 0.8264163372859025]</t>
         </is>
       </c>
     </row>
@@ -2051,14 +2051,14 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.8247732858716841</v>
+        <v>0.8324706694271912</v>
       </c>
       <c r="E58" t="n">
-        <v>0.02548106381591808</v>
+        <v>0.02636261025711029</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[0.82, 0.8278667683702009, 0.8494252873563217, 0.8507804921068877, 0.8216798033731673, 0.8336483931947071, 0.8093944099378882, 0.82, 0.8764976958525345, 0.8100739839870275]</t>
+          <t>[0.8388543823326432, 0.8388543823326432, 0.8494252873563217, 0.8622222222222221, 0.8216798033731673, 0.8260869565217391, 0.8093944099378882, 0.82, 0.8764976958525345, 0.8100739839870275]</t>
         </is>
       </c>
     </row>
@@ -2082,11 +2082,11 @@
         <v>0.8043478260869565</v>
       </c>
       <c r="E59" t="n">
-        <v>0.0240338164251207</v>
+        <v>0.01666666666666661</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[0.8, 0.8260869565217391, 0.8222222222222222, 0.8260869565217391, 0.8043478260869565, 0.782608695652174, 0.8043478260869565, 0.8, 0.8666666666666667, 0.8043478260869565]</t>
+          <t>[0.8043478260869565, 0.8043478260869565, 0.8222222222222222, 0.8444444444444444, 0.8, 0.782608695652174, 0.8043478260869565, 0.8, 0.8666666666666667, 0.8043478260869565]</t>
         </is>
       </c>
     </row>
@@ -2107,14 +2107,14 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.8245920745920746</v>
+        <v>0.8371026440879382</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0266029925956397</v>
+        <v>0.02119755244755239</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>[0.7983682983682983, 0.8205128205128206, 0.8484848484848484, 0.8088578088578088, 0.8396464646464646, 0.824009324009324, 0.8251748251748252, 0.7692307692307693, 0.8876262626262627, 0.8345588235294118]</t>
+          <t>[0.8005050505050504, 0.8263403263403264, 0.8671328671328672, 0.8473193473193473, 0.8396464646464646, 0.8446969696969697, 0.8251748251748252, 0.7692307692307693, 0.8876262626262627, 0.8345588235294118]</t>
         </is>
       </c>
     </row>
@@ -2135,14 +2135,14 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.8066333882427328</v>
+        <v>0.8094542371031742</v>
       </c>
       <c r="E61" t="n">
-        <v>0.02088972568924707</v>
+        <v>0.01853792058997472</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[0.8063492063492064, 0.8213981244671781, 0.8291858678955453, 0.8320710612435719, 0.8063492063492064, 0.7900888265544647, 0.8064659977703456, 0.8063492063492064, 0.8697115384615384, 0.80680077871512]</t>
+          <t>[0.8121076954912284, 0.8121076954912284, 0.8291858678955453, 0.8493827160493829, 0.8063492063492064, 0.7900888265544647, 0.8064659977703456, 0.8063492063492064, 0.8697115384615384, 0.80680077871512]</t>
         </is>
       </c>
     </row>
@@ -2163,14 +2163,14 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.7423312691854891</v>
+        <v>0.7508564166407303</v>
       </c>
       <c r="E62" t="n">
-        <v>0.03152576495361648</v>
+        <v>0.01876384755082083</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>[0.7439427722036417, 0.7407197661673365, 0.7752305665349144, 0.7202053617460045, 0.757905982905983, 0.7600414078674949, 0.7020626432391139, 0.7187301587301587, 0.7492945326278659, 0.7362933362933363]</t>
+          <t>[0.7399682075958067, 0.7407197661673365, 0.7712760161272747, 0.7202053617460045, 0.7555555555555555, 0.7600414078674949, 0.7524183006535948, 0.6625656951743908, 0.7492945326278659, 0.7773386034255599]</t>
         </is>
       </c>
     </row>
@@ -2191,14 +2191,14 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.6922705314009662</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="E63" t="n">
-        <v>0.03804347826086951</v>
+        <v>0.04999999999999993</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>[0.6521739130434783, 0.6739130434782609, 0.7391304347826086, 0.6666666666666666, 0.6956521739130435, 0.7391304347826086, 0.6956521739130435, 0.6888888888888889, 0.6739130434782609, 0.717391304347826]</t>
+          <t>[0.6521739130434783, 0.6739130434782609, 0.7391304347826086, 0.6956521739130435, 0.7333333333333333, 0.7391304347826086, 0.6956521739130435, 0.6739130434782609, 0.6739130434782609, 0.6956521739130435]</t>
         </is>
       </c>
     </row>
@@ -2219,14 +2219,14 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.8310958074805832</v>
+        <v>0.8318412137062021</v>
       </c>
       <c r="E64" t="n">
-        <v>0.02300268752213819</v>
+        <v>0.03035421989941445</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[0.7690260730878581, 0.8327439151237777, 0.8194473337493932, 0.8321148721606386, 0.8483696890447463, 0.8615721616293699, 0.8300767428005279, 0.798237783237783, 0.8397579397579397, 0.8135198835198836]</t>
+          <t>[0.7729372595101495, 0.8335475546573944, 0.8194473337493932, 0.83013487275501, 0.8456516786036237, 0.8615721616293699, 0.80016865285744, 0.8119495874072532, 0.8397579397579397, 0.8666416535409671]</t>
         </is>
       </c>
     </row>
@@ -2247,14 +2247,14 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.6988407191305743</v>
+        <v>0.6989943102487346</v>
       </c>
       <c r="E65" t="n">
-        <v>0.02071639264704395</v>
+        <v>0.04007863976266424</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[0.6684265010351967, 0.6915239350021958, 0.7426326627059142, 0.6992710992710993, 0.6994565217391305, 0.7439988597833589, 0.6930928152944805, 0.6984103389900492, 0.6928400962779123, 0.7183407176590876]</t>
+          <t>[0.6603777920764776, 0.6915239350021958, 0.7426326627059142, 0.7048958052029886, 0.7386762459226228, 0.7439988597833589, 0.6930928152944805, 0.6678601875532821, 0.6928400962779123, 0.7116977225672878]</t>
         </is>
       </c>
     </row>
@@ -2275,14 +2275,14 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.8555049216767138</v>
+        <v>0.8561446918817013</v>
       </c>
       <c r="E66" t="n">
-        <v>0.02143470088264132</v>
+        <v>0.02318375195234457</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[0.8594202898550726, 0.8361801242236023, 0.8570048309178743, 0.8361801242236023, 0.8372598162071847, 0.8846235418875928, 0.8581780538302277, 0.8557252905078991, 0.8342391304347826, 0.8552845528455284]</t>
+          <t>[0.8594202898550726, 0.8232804232804232, 0.8570048309178743, 0.8372598162071847, 0.8342391304347826, 0.8581780538302277, 0.8581780538302277, 0.8845410628019322, 0.8267610380856084, 0.8552845528455284]</t>
         </is>
       </c>
     </row>
@@ -2303,14 +2303,14 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.8478260869565217</v>
+        <v>0.8572463768115942</v>
       </c>
       <c r="E67" t="n">
-        <v>0.02101449275362322</v>
+        <v>0.02427536231884064</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[0.8695652173913043, 0.8444444444444444, 0.8260869565217391, 0.8478260869565217, 0.8478260869565217, 0.8695652173913043, 0.8695652173913043, 0.8478260869565217, 0.8478260869565217, 0.8666666666666667]</t>
+          <t>[0.8695652173913043, 0.8444444444444444, 0.8260869565217391, 0.8444444444444444, 0.8478260869565217, 0.8695652173913043, 0.8695652173913043, 0.8695652173913043, 0.8478260869565217, 0.8666666666666667]</t>
         </is>
       </c>
     </row>
@@ -2331,14 +2331,14 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.853978978978979</v>
+        <v>0.8476222933459776</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0523648648648648</v>
+        <v>0.05749911095305837</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[0.8498498498498499, 0.8310810810810811, 0.8918918918918919, 0.7939189189189189, 0.8614864864864865, 0.8581081081081081, 0.9358108108108109, 0.9054054054054054, 0.8344594594594594, 0.8277027027027027]</t>
+          <t>[0.8453947368421053, 0.8074324324324325, 0.8498498498498499, 0.8277027027027026, 0.8817567567567568, 0.8651315789473685, 0.9324324324324325, 0.8885135135135136, 0.8175675675675675, 0.8006756756756757]</t>
         </is>
       </c>
     </row>
@@ -2362,11 +2362,11 @@
         <v>0.8410720611916264</v>
       </c>
       <c r="E69" t="n">
-        <v>0.0239462053425199</v>
+        <v>0.02643051895769277</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[0.8588972431077694, 0.8233775030693028, 0.8158942506768594, 0.8233775030693028, 0.8402962962962963, 0.8418478260869564, 0.851086956521739, 0.8512872975277067, 0.8352067868504772, 0.8478632478632478]</t>
+          <t>[0.8418478260869564, 0.8140135532540596, 0.8158942506768594, 0.8402962962962963, 0.8355731225296441, 0.851086956521739, 0.851086956521739, 0.8671525380386138, 0.817937832430586, 0.8418478260869564]</t>
         </is>
       </c>
     </row>
@@ -2387,14 +2387,14 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.8189229249011858</v>
+        <v>0.8096061547148503</v>
       </c>
       <c r="E70" t="n">
-        <v>0.02050250343019733</v>
+        <v>0.03606355029409947</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[0.826526130873957, 0.8117588932806324, 0.8025210084033613, 0.8074534161490682, 0.8298676748582231, 0.8117588932806324, 0.8443544759334234, 0.8260869565217391, 0.8458994708994709, 0.7863894139886578]</t>
+          <t>[0.826526130873957, 0.8047683310841206, 0.8025210084033613, 0.8074534161490682, 0.8056653491436101, 0.8117588932806324, 0.8683127572016461, 0.8479096989966556, 0.8458994708994709, 0.7863894139886578]</t>
         </is>
       </c>
     </row>
@@ -2415,14 +2415,14 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.8132850241545894</v>
+        <v>0.8043478260869565</v>
       </c>
       <c r="E71" t="n">
-        <v>0.02173913043478259</v>
+        <v>0.03454106280193225</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>[0.8222222222222222, 0.8043478260869565, 0.782608695652174, 0.8043478260869565, 0.8260869565217391, 0.8043478260869565, 0.8444444444444444, 0.8260869565217391, 0.8444444444444444, 0.7777777777777778]</t>
+          <t>[0.8222222222222222, 0.8043478260869565, 0.782608695652174, 0.8043478260869565, 0.8043478260869565, 0.8043478260869565, 0.8666666666666667, 0.8478260869565217, 0.8444444444444444, 0.782608695652174]</t>
         </is>
       </c>
     </row>
@@ -2443,14 +2443,14 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.908</v>
+        <v>0.9170952380952382</v>
       </c>
       <c r="E72" t="n">
-        <v>0.01999999999999991</v>
+        <v>0.01952380952380972</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>[0.898, 0.9142857142857143, 0.8914285714285715, 0.906, 0.906, 0.9276190476190477, 0.9279999999999999, 0.9219047619047619, 0.91, 0.888]</t>
+          <t>[0.894, 0.9161904761904762, 0.89, 0.918, 0.9059999999999999, 0.9180952380952381, 0.9238095238095239, 0.9219047619047619, 0.92, 0.8979999999999999]</t>
         </is>
       </c>
     </row>
@@ -2471,14 +2471,14 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.8136883348261701</v>
+        <v>0.8046258737559089</v>
       </c>
       <c r="E73" t="n">
-        <v>0.02340760425583199</v>
+        <v>0.03651340531109459</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[0.8227513227513227, 0.8046253469010175, 0.7813735177865612, 0.8023600681517005, 0.8264163372859025, 0.8046253469010175, 0.8439751969163732, 0.8260869565217391, 0.8447541618273327, 0.777119016249451]</t>
+          <t>[0.8227513227513227, 0.8038799825338406, 0.7813735177865612, 0.8023600681517005, 0.8046264006108004, 0.8046253469010175, 0.8657219973009447, 0.8474622086374317, 0.8447541618273327, 0.7813545150501673]</t>
         </is>
       </c>
     </row>
@@ -2502,11 +2502,11 @@
         <v>0.8675675675675676</v>
       </c>
       <c r="E74" t="n">
-        <v>0.002828200053600405</v>
+        <v>0.002399138268703416</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>[0.8716542629586108, 0.8675675675675676, 0.8888888888888888, 0.8666666666666667, 0.8666666666666667, 0.8675675675675676, 0.8443817052512704, 0.8666290231507624, 0.870137299771167, 0.8675675675675676]</t>
+          <t>[0.8716542629586108, 0.8675675675675676, 0.8675675675675676, 0.8666666666666667, 0.8666666666666667, 0.843840579710145, 0.8443817052512704, 0.8695652173913043, 0.870137299771167, 0.8675675675675676]</t>
         </is>
       </c>
     </row>
@@ -2530,11 +2530,11 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="E75" t="n">
-        <v>0.002898550724637627</v>
+        <v>0.002173913043478248</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[0.8695652173913043, 0.8666666666666667, 0.8695652173913043, 0.8666666666666667, 0.8666666666666667, 0.8666666666666667, 0.8478260869565217, 0.8695652173913043, 0.8695652173913043, 0.8666666666666667]</t>
+          <t>[0.8695652173913043, 0.8666666666666667, 0.8666666666666667, 0.8666666666666667, 0.8666666666666667, 0.8444444444444444, 0.8478260869565217, 0.8695652173913043, 0.8695652173913043, 0.8666666666666667]</t>
         </is>
       </c>
     </row>
@@ -2555,14 +2555,14 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.9017094017094017</v>
+        <v>0.9008352758352758</v>
       </c>
       <c r="E76" t="n">
-        <v>0.02027629233511585</v>
+        <v>0.03292540792540799</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[0.9277389277389277, 0.898989898989899, 0.8939393939393939, 0.9044289044289044, 0.9090909090909091, 0.892156862745098, 0.914141414141414, 0.8823529411764706, 0.9338235294117647, 0.8636363636363636]</t>
+          <t>[0.9207459207459208, 0.8838383838383839, 0.8951048951048951, 0.923076923076923, 0.909090909090909, 0.9065656565656566, 0.8881118881118881, 0.8813131313131313, 0.9240196078431373, 0.8636363636363636]</t>
         </is>
       </c>
     </row>
@@ -2586,11 +2586,11 @@
         <v>0.8586438923395445</v>
       </c>
       <c r="E77" t="n">
-        <v>0.009033198259540964</v>
+        <v>0.008359213250517694</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[0.8660485933503835, 0.8571428571428571, 0.8554347826086957, 0.8614342179559572, 0.8666666666666667, 0.8571428571428571, 0.845620667926906, 0.8660485933503835, 0.860144927536232, 0.85]</t>
+          <t>[0.860144927536232, 0.8571428571428571, 0.8571428571428571, 0.8614342179559572, 0.8666666666666667, 0.8367149758454108, 0.845620667926906, 0.860144927536232, 0.860144927536232, 0.85]</t>
         </is>
       </c>
     </row>
@@ -2611,14 +2611,14 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.7587767425810903</v>
+        <v>0.7316551906225819</v>
       </c>
       <c r="E78" t="n">
-        <v>0.03522322663251698</v>
+        <v>0.04016791311581436</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[0.7414596273291927, 0.7622630992196211, 0.7713962711738759, 0.7247234247234247, 0.779014262709915, 0.6979010494752622, 0.7594444444444444, 0.7313664596273292, 0.7933684672815108, 0.7581090407177363]</t>
+          <t>[0.7195681005651021, 0.7006979787698124, 0.6913521261347348, 0.7247234247234247, 0.7945849297573435, 0.7247234247234247, 0.7618357487922707, 0.7585921325051759, 0.7970899470899471, 0.7385869565217391]</t>
         </is>
       </c>
     </row>
@@ -2639,14 +2639,14 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.7582125603864734</v>
+        <v>0.7362318840579709</v>
       </c>
       <c r="E79" t="n">
-        <v>0.02173913043478271</v>
+        <v>0.03405797101449271</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[0.7391304347826086, 0.7608695652173914, 0.7608695652173914, 0.7333333333333333, 0.782608695652174, 0.7111111111111111, 0.7608695652173914, 0.7391304347826086, 0.7777777777777778, 0.7555555555555555]</t>
+          <t>[0.717391304347826, 0.6956521739130435, 0.6956521739130435, 0.7333333333333333, 0.8, 0.7333333333333333, 0.7608695652173914, 0.7391304347826086, 0.7777777777777778, 0.7391304347826086]</t>
         </is>
       </c>
     </row>
@@ -2667,14 +2667,14 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.8721891190426661</v>
+        <v>0.882483355149259</v>
       </c>
       <c r="E80" t="n">
-        <v>0.01818507134801406</v>
+        <v>0.03075945751776965</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>[0.8699887069452288, 0.8664473564473565, 0.8584851456705004, 0.88502877747729, 0.9120380001386866, 0.8413137287817595, 0.9184474024627477, 0.8743895311401032, 0.8661230649721697, 0.8824705043240513]</t>
+          <t>[0.8820256620256619, 0.8656013521742421, 0.8397277779428809, 0.8727700427700427, 0.9142371739625744, 0.8593621937611706, 0.9184194241738999, 0.8879170079170079, 0.882941048272856, 0.9015649738156132]</t>
         </is>
       </c>
     </row>
@@ -2695,14 +2695,14 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.7550887091442875</v>
+        <v>0.7301189698043435</v>
       </c>
       <c r="E81" t="n">
-        <v>0.03781632202322471</v>
+        <v>0.03558123937593616</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[0.7220925096232725, 0.7610470275066549, 0.7595238095238096, 0.7251220750810577, 0.7792865105908583, 0.697119341563786, 0.7568979933110368, 0.7162939603464623, 0.7614729370008873, 0.7532794249775381]</t>
+          <t>[0.7151368760064413, 0.6969088482074753, 0.692924126172208, 0.7251220750810577, 0.7905082571749239, 0.7251220750810577, 0.7591213134691396, 0.7351158645276292, 0.7795721187025535, 0.7354937201967072]</t>
         </is>
       </c>
     </row>
@@ -2723,14 +2723,14 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.8595943116621803</v>
+        <v>0.8647225167903854</v>
       </c>
       <c r="E82" t="n">
-        <v>0.02582107851405169</v>
+        <v>0.008178053830227849</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>[0.8372598162071847, 0.8627783669141039, 0.8877654196157734, 0.8140749445097272, 0.8695652173913043, 0.8627783669141039, 0.8564102564102565, 0.9071225071225071, 0.8296924708377518, 0.8564102564102565]</t>
+          <t>[0.8666666666666667, 0.8594202898550726, 0.8666666666666667, 0.8372598162071847, 0.8666666666666667, 0.8581780538302277, 0.8842940685045949, 0.8557252905078991, 0.8695652173913043, 0.8627783669141039]</t>
         </is>
       </c>
     </row>
@@ -2751,14 +2751,14 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.8572463768115942</v>
       </c>
       <c r="E83" t="n">
-        <v>0.02427536231884064</v>
+        <v>0.02101449275362322</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[0.8444444444444444, 0.8695652173913043, 0.8695652173913043, 0.8260869565217391, 0.8695652173913043, 0.8478260869565217, 0.8666666666666667, 0.9111111111111111, 0.8260869565217391, 0.8666666666666667]</t>
+          <t>[0.8666666666666667, 0.8695652173913043, 0.8478260869565217, 0.8444444444444444, 0.8666666666666667, 0.8695652173913043, 0.8888888888888888, 0.8478260869565217, 0.8478260869565217, 0.8478260869565217]</t>
         </is>
       </c>
     </row>
@@ -2779,14 +2779,14 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.8410433459775566</v>
+        <v>0.8716216216216217</v>
       </c>
       <c r="E84" t="n">
-        <v>0.05263404852220654</v>
+        <v>0.05307857199304566</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>[0.8322368421052632, 0.8277027027027026, 0.8498498498498499, 0.8243243243243243, 0.8708708708708709, 0.888157894736842, 0.8888888888888888, 0.8848684210526316, 0.8318318318318317, 0.8092105263157895]</t>
+          <t>[0.8453947368421053, 0.8682432432432433, 0.9054054054054054, 0.8243243243243243, 0.8851351351351351, 0.875, 0.9358108108108107, 0.9210526315789473, 0.8528528528528528, 0.8289473684210527]</t>
         </is>
       </c>
     </row>
@@ -2807,14 +2807,14 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.8538574599231447</v>
+        <v>0.8558015253667428</v>
       </c>
       <c r="E85" t="n">
-        <v>0.01821306436380798</v>
+        <v>0.01002778500944479</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[0.8402962962962963, 0.8542761586239848, 0.8418478260869564, 0.8175057208237987, 0.8695652173913043, 0.8534387612223046, 0.8588972431077694, 0.9059314954051797, 0.8260869565217391, 0.8588972431077694]</t>
+          <t>[0.8588972431077694, 0.8619206880076445, 0.8260869565217391, 0.8352067868504772, 0.8666666666666667, 0.851086956521739, 0.8859259259259259, 0.8512872975277067, 0.8573268921095009, 0.8542761586239848]</t>
         </is>
       </c>
     </row>
@@ -2835,14 +2835,14 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.848485481909395</v>
+        <v>0.8504740460404077</v>
       </c>
       <c r="E86" t="n">
-        <v>0.01049707173706027</v>
+        <v>0.01596134843417452</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>[0.8479096989966556, 0.8683127572016461, 0.8074534161490682, 0.8511021142600089, 0.8490612648221345, 0.8764367816091954, 0.8298676748582231, 0.8386749482401656, 0.8443544759334234, 0.8490612648221345]</t>
+          <t>[0.8056653491436101, 0.8683127572016461, 0.8530383930841596, 0.8479096989966556, 0.8479096989966556, 0.8944911297852474, 0.8666666666666667, 0.8554841897233202, 0.8298676748582231, 0.8479096989966556]</t>
         </is>
       </c>
     </row>
@@ -2863,14 +2863,14 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.8478260869565217</v>
       </c>
       <c r="E87" t="n">
-        <v>0.02173913043478259</v>
+        <v>0.0304347826086957</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>[0.8478260869565217, 0.8666666666666667, 0.8043478260869565, 0.8260869565217391, 0.8444444444444444, 0.8666666666666667, 0.8260869565217391, 0.8260869565217391, 0.8444444444444444, 0.8478260869565217]</t>
+          <t>[0.8043478260869565, 0.8666666666666667, 0.8260869565217391, 0.8478260869565217, 0.8478260869565217, 0.8888888888888888, 0.8666666666666667, 0.8478260869565217, 0.8260869565217391, 0.8478260869565217]</t>
         </is>
       </c>
     </row>
@@ -2891,14 +2891,14 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.9152380952380952</v>
+        <v>0.9258571428571428</v>
       </c>
       <c r="E88" t="n">
-        <v>0.01654761904761914</v>
+        <v>0.02000000000000002</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[0.9161904761904762, 0.9142857142857143, 0.8904761904761905, 0.9140000000000001, 0.9085714285714286, 0.9390476190476189, 0.928, 0.9104761904761904, 0.9276190476190476, 0.940952380952381]</t>
+          <t>[0.8980000000000001, 0.9352380952380952, 0.9295238095238095, 0.8838095238095238, 0.9104761904761904, 0.9520000000000001, 0.9259999999999999, 0.9257142857142857, 0.948, 0.9238095238095237]</t>
         </is>
       </c>
     </row>
@@ -2919,14 +2919,14 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.8432579253888908</v>
+        <v>0.8474622086374317</v>
       </c>
       <c r="E89" t="n">
-        <v>0.02172831746954496</v>
+        <v>0.02962417697156605</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[0.8474622086374317, 0.8657219973009447, 0.8046264006108004, 0.8250836120401338, 0.8425406538614084, 0.8641975308641976, 0.8264163372859025, 0.8260869565217391, 0.8439751969163732, 0.8480427560306225]</t>
+          <t>[0.8046264006108004, 0.8657219973009447, 0.8260869565217391, 0.8474622086374317, 0.8474622086374317, 0.8875290384724346, 0.8666666666666667, 0.8480419364785693, 0.8264163372859025, 0.8474622086374317]</t>
         </is>
       </c>
     </row>
@@ -2947,14 +2947,14 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.8574281832298136</v>
+        <v>0.8446652771780649</v>
       </c>
       <c r="E90" t="n">
-        <v>0.02370436135142029</v>
+        <v>0.02268475476995291</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[0.8519992236024845, 0.8152380952380952, 0.8716542629586108, 0.8926282051282052, 0.8628571428571429, 0.8409982174688057, 0.8657004830917875, 0.8628571428571429, 0.8421464943204073, 0.8337941628264208]</t>
+          <t>[0.8491987179487179, 0.8443817052512704, 0.8378151260504202, 0.9044444444444444, 0.8792701863354037, 0.8222222222222222, 0.8525387655822437, 0.8260869565217391, 0.8449488491048593, 0.8093944099378882]</t>
         </is>
       </c>
     </row>
@@ -2975,14 +2975,14 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.8572463768115942</v>
+        <v>0.8352657004830918</v>
       </c>
       <c r="E91" t="n">
-        <v>0.02355072463768126</v>
+        <v>0.02173913043478259</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[0.8478260869565217, 0.8222222222222222, 0.8695652173913043, 0.8888888888888888, 0.8666666666666667, 0.8444444444444444, 0.8695652173913043, 0.8666666666666667, 0.8478260869565217, 0.8260869565217391]</t>
+          <t>[0.8444444444444444, 0.8260869565217391, 0.8260869565217391, 0.8913043478260869, 0.8695652173913043, 0.8222222222222222, 0.8478260869565217, 0.8260869565217391, 0.8478260869565217, 0.8043478260869565]</t>
         </is>
       </c>
     </row>
@@ -3003,14 +3003,14 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.9025835275835276</v>
+        <v>0.9031662781662781</v>
       </c>
       <c r="E92" t="n">
-        <v>0.02616378719319901</v>
+        <v>0.01951071804012983</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>[0.9324009324009324, 0.8897058823529411, 0.9142156862745097, 0.9671717171717171, 0.8904428904428905, 0.8787878787878788, 0.8914141414141414, 0.8863636363636364, 0.9137529137529137, 0.9166666666666666]</t>
+          <t>[0.898989898989899, 0.9191919191919192, 0.9117647058823529, 0.9533799533799534, 0.9343434343434343, 0.8578088578088578, 0.9065656565656566, 0.8737373737373737, 0.8974358974358974, 0.8997668997668997]</t>
         </is>
       </c>
     </row>
@@ -3031,14 +3031,14 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0.8554538858886686</v>
+        <v>0.8380295542657644</v>
       </c>
       <c r="E93" t="n">
-        <v>0.02188233117497673</v>
+        <v>0.02570179204312861</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>[0.8494735538213799, 0.8167557932263816, 0.8614342179559572, 0.8902564102564102, 0.8625668449197861, 0.8422236642872594, 0.8654997176736307, 0.8625668449197861, 0.8401714635639926, 0.8262820512820512]</t>
+          <t>[0.8463589743589742, 0.8213981244671781, 0.8301408736191344, 0.8924811098724141, 0.8726056552143507, 0.8222222222222222, 0.8497339390006488, 0.8260869565217391, 0.8459182349123945, 0.8064659977703456]</t>
         </is>
       </c>
     </row>
@@ -3059,14 +3059,14 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.7585685751446622</v>
+        <v>0.7668531468531469</v>
       </c>
       <c r="E94" t="n">
-        <v>0.01552337382231661</v>
+        <v>0.0301162818426246</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>[0.7639751552795032, 0.7193415637860081, 0.730936065352417, 0.7533947312058256, 0.7683326399001456, 0.7539682539682541, 0.8165079365079366, 0.751161616161616, 0.7631688963210703, 0.782608695652174]</t>
+          <t>[0.7450076209667003, 0.7333333333333333, 0.7259316770186335, 0.7710800310800311, 0.7596153846153846, 0.7626262626262627, 0.7729096989966555, 0.7867599067599068, 0.8050724637681159, 0.7807312252964427]</t>
         </is>
       </c>
     </row>
@@ -3087,14 +3087,14 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>0.7391304347826086</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="E95" t="n">
-        <v>0.0260869565217392</v>
+        <v>0.02077294685990339</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[0.7608695652173914, 0.7333333333333333, 0.717391304347826, 0.7391304347826086, 0.7391304347826086, 0.7391304347826086, 0.8222222222222222, 0.7333333333333333, 0.7608695652173914, 0.7608695652173914]</t>
+          <t>[0.6956521739130435, 0.7333333333333333, 0.7333333333333333, 0.7555555555555555, 0.7555555555555555, 0.7555555555555555, 0.7608695652173914, 0.7555555555555555, 0.7777777777777778, 0.7391304347826086]</t>
         </is>
       </c>
     </row>
@@ -3115,14 +3115,14 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>0.9031059967215573</v>
+        <v>0.8932132132132132</v>
       </c>
       <c r="E96" t="n">
-        <v>0.02327698923573196</v>
+        <v>0.01373291015167433</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>[0.8914771549042648, 0.9157484757484758, 0.8921736158578264, 0.8959150059150058, 0.9322045231656214, 0.8919028119028118, 0.9137445812637629, 0.8769007498984616, 0.9282564382564383, 0.9102969875281088]</t>
+          <t>[0.8746664846664847, 0.8932532532532532, 0.895744796774545, 0.8931731731731732, 0.9003858460380201, 0.8837073437073438, 0.8989073474199332, 0.8618209118209118, 0.9130137596956819, 0.8864131673056158]</t>
         </is>
       </c>
     </row>
@@ -3143,14 +3143,14 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0.7445364812591704</v>
+        <v>0.7569142207607681</v>
       </c>
       <c r="E97" t="n">
-        <v>0.02093230981231831</v>
+        <v>0.02267963579933507</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[0.7594063545150501, 0.7240537240537239, 0.7210644677661169, 0.7474632751651384, 0.7416096873532022, 0.7396181716833891, 0.8156025665459626, 0.7407100682463003, 0.7612958226768969, 0.7652638088728314]</t>
+          <t>[0.7032284959111632, 0.7333333333333333, 0.729201921950076, 0.7596910953506698, 0.7570793650793651, 0.756749076442171, 0.7702075702075701, 0.7604938271604939, 0.7832347753916382, 0.7504540336348116]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated model metrics with dataset v10
</commit_message>
<xml_diff>
--- a/data/processed/model_metrics_comparison_with_raw.xlsx
+++ b/data/processed/model_metrics_comparison_with_raw.xlsx
@@ -483,14 +483,14 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.8564102564102565</v>
+        <v>0.867343942407881</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02585148289228212</v>
+        <v>0.02233914211022126</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[0.8695652173913043, 0.8627783669141039, 0.8877654196157734, 0.8372598162071847, 0.8564102564102565, 0.8372598162071847, 0.8564102564102565, 0.8822222222222222, 0.8267610380856084, 0.8562886388973346]</t>
+          <t>[0.8494809688581315, 0.872005323868678, 0.8811690714021457, 0.8609385783298826, 0.855072463768116, 0.8677654636733921, 0.8669224211423701, 0.8434486838213546, 0.8990808823529413, 0.8823529411764706]</t>
         </is>
       </c>
     </row>
@@ -511,14 +511,14 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.8623188405797102</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0170289855072463</v>
+        <v>0.0256820119352088</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[0.8695652173913043, 0.8695652173913043, 0.8695652173913043, 0.8444444444444444, 0.8666666666666667, 0.8444444444444444, 0.8666666666666667, 0.8695652173913043, 0.8478260869565217, 0.8666666666666667]</t>
+          <t>[0.8529411764705882, 0.8695652173913043, 0.8823529411764706, 0.855072463768116, 0.855072463768116, 0.8695652173913043, 0.8529411764705882, 0.8405797101449275, 0.8970588235294118, 0.8823529411764706]</t>
         </is>
       </c>
     </row>
@@ -539,14 +539,14 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.8597972972972974</v>
+        <v>0.9290816326530613</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05515795400663825</v>
+        <v>0.02089151450053683</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[0.8782894736842105, 0.8228228228228227, 0.9155405405405406, 0.8209459459459458, 0.8888888888888888, 0.8716216216216216, 0.9189189189189189, 0.847972972972973, 0.8288288288288288, 0.8378378378378378]</t>
+          <t>[0.9336842105263157, 0.9084210526315789, 0.9431578947368421, 0.9275510204081632, 0.911578947368421, 0.9173469387755102, 0.9285714285714286, 0.929591836734694, 0.949516648764769, 0.9452201933404941]</t>
         </is>
       </c>
     </row>
@@ -567,14 +567,14 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8565867008658771</v>
+        <v>0.8628325508514304</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01897679259464147</v>
+        <v>0.02044105799719442</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[0.8695652173913043, 0.8542761586239848, 0.8619206880076445, 0.8402962962962963, 0.8588972431077694, 0.8402962962962963, 0.8588972431077694, 0.8782328782328783, 0.817937832430586, 0.8478632478632478]</t>
+          <t>[0.8503267973856209, 0.8705786966656531, 0.8777393310265282, 0.8572167997633836, 0.855072463768116, 0.8684483019394772, 0.8568150664521127, 0.8418184070357985, 0.8978479575811292, 0.8823529411764706]</t>
         </is>
       </c>
     </row>
@@ -595,14 +595,14 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.8415147120867945</v>
+        <v>0.8547452973284175</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03051767401595762</v>
+        <v>0.02391205187290746</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[0.8458994708994709, 0.8386749482401656, 0.8443544759334234, 0.8655555555555556, 0.827273497754047, 0.8056653491436101, 0.8683127572016461, 0.8386749482401656, 0.8683127572016461, 0.8260869565217391]</t>
+          <t>[0.8410668615272195, 0.8146684233640756, 0.8404798761609906, 0.8823529411764706, 0.8681945505474918, 0.855072463768116, 0.8559090573558722, 0.8412990196078431, 0.8680795847750865, 0.8544181308887192]</t>
         </is>
       </c>
     </row>
@@ -623,14 +623,14 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.8352657004830918</v>
+        <v>0.854006820119352</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01835748792270531</v>
+        <v>0.0256820119352088</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[0.8444444444444444, 0.8260869565217391, 0.8444444444444444, 0.8444444444444444, 0.8260869565217391, 0.8043478260869565, 0.8666666666666667, 0.8260869565217391, 0.8666666666666667, 0.8260869565217391]</t>
+          <t>[0.8405797101449275, 0.8115942028985508, 0.8382352941176471, 0.8823529411764706, 0.8676470588235294, 0.855072463768116, 0.855072463768116, 0.8382352941176471, 0.8676470588235294, 0.8529411764705882]</t>
         </is>
       </c>
     </row>
@@ -651,14 +651,14 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.9247619047619047</v>
+        <v>0.9217171717171717</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01690476190476187</v>
+        <v>0.01356383778258774</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[0.9179999999999999, 0.918, 0.9180952380952381, 0.9066666666666666, 0.939047619047619, 0.937142857142857, 0.934, 0.9314285714285714, 0.9352380952380952, 0.9180952380952381]</t>
+          <t>[0.9158249158249158, 0.9208754208754208, 0.9307359307359307, 0.9419913419913419, 0.936026936026936, 0.9132996632996633, 0.9158249158249159, 0.915798611111111, 0.9225589225589226, 0.9253472222222223]</t>
         </is>
       </c>
     </row>
@@ -679,14 +679,14 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.8350310767190562</v>
+        <v>0.8538538138522154</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01858977595987144</v>
+        <v>0.02563662631333807</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[0.8447541618273327, 0.8260869565217391, 0.8439751969163732, 0.8444444444444444, 0.8250836120401338, 0.8046264006108004, 0.8657219973009447, 0.8260869565217391, 0.8657219973009447, 0.8260869565217391]</t>
+          <t>[0.8406467357029915, 0.8115942028985508, 0.8377076858140516, 0.8823529411764706, 0.8677330954050092, 0.855072463768116, 0.8547664512338425, 0.8381303202656794, 0.8675039126617552, 0.8529411764705882]</t>
         </is>
       </c>
     </row>
@@ -707,14 +707,14 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.8386851769905972</v>
+        <v>0.9043927217138998</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02548078923455321</v>
+        <v>0.01387497809931071</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[0.8363721365123888, 0.8657004830917875, 0.8896321070234113, 0.8222826086956523, 0.8409982174688057, 0.8337941628264208, 0.8449488491048593, 0.8222222222222222, 0.8204404291360813, 0.8525387655822437]</t>
+          <t>[0.9100046750818139, 0.8977455716586151, 0.920443587270974, 0.8977455716586151, 0.8920385395537526, 0.9100046750818139, 0.8987807683459857, 0.8952205882352942, 0.9121591746499632, 0.920443587270974]</t>
         </is>
       </c>
     </row>
@@ -735,14 +735,14 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.8352657004830918</v>
+        <v>0.8985507246376812</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02173913043478259</v>
+        <v>0.01102941176470584</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[0.8260869565217391, 0.8695652173913043, 0.8695652173913043, 0.8043478260869565, 0.8444444444444444, 0.8260869565217391, 0.8478260869565217, 0.8260869565217391, 0.8260869565217391, 0.8478260869565217]</t>
+          <t>[0.8985507246376812, 0.8985507246376812, 0.9117647058823529, 0.8985507246376812, 0.8970588235294118, 0.8985507246376812, 0.8970588235294118, 0.8970588235294118, 0.9130434782608695, 0.9117647058823529]</t>
         </is>
       </c>
     </row>
@@ -763,14 +763,14 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.8898601398601398</v>
+        <v>0.881168831168831</v>
       </c>
       <c r="E12" t="n">
-        <v>0.03773310023310017</v>
+        <v>0.03671328671328666</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[0.8676470588235294, 0.8712121212121212, 0.9141414141414141, 0.9166666666666666, 0.8857808857808858, 0.8686868686868687, 0.9114219114219114, 0.8939393939393939, 0.8529411764705882, 0.893939393939394]</t>
+          <t>[0.8573426573426574, 0.8937062937062936, 0.8965034965034965, 0.8344155844155844, 0.8896103896103895, 0.8643356643356643, 0.9300699300699301, 0.8551948051948052, 0.8727272727272727, 0.9064935064935066]</t>
         </is>
       </c>
     </row>
@@ -791,14 +791,14 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.8359022048144371</v>
+        <v>0.8897290485192186</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02554283349140563</v>
+        <v>0.01099900816855015</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[0.8295807453416149, 0.8654997176736307, 0.8695652173913043, 0.809809381023774, 0.8422236642872594, 0.8262820512820512, 0.8459182349123945, 0.8222222222222222, 0.8213981244671781, 0.8497339390006488]</t>
+          <t>[0.8846773194599282, 0.8897290485192186, 0.9008113590263692, 0.8897290485192186, 0.8897290485192186, 0.8846773194599282, 0.8870417732310315, 0.8870417732310315, 0.9073226544622426, 0.9008113590263692]</t>
         </is>
       </c>
     </row>
@@ -819,14 +819,14 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.7697736625514404</v>
+        <v>0.7927393320548524</v>
       </c>
       <c r="E14" t="n">
-        <v>0.009746319170037543</v>
+        <v>0.007081354135822893</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[0.7710640021604105, 0.7790361812100942, 0.7453416149068323, 0.7695473251028807, 0.8222222222222222, 0.77, 0.8059356102834363, 0.768888888888889, 0.7667661267405512, 0.757996894409938]</t>
+          <t>[0.7919439268920236, 0.7918056009589189, 0.8088235294117647, 0.7761674718196457, 0.7920350748995251, 0.8002760524499655, 0.8083466627890068, 0.7948579889621752, 0.7934435892101795, 0.7714786397650848]</t>
         </is>
       </c>
     </row>
@@ -847,14 +847,14 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.7693236714975846</v>
+        <v>0.7956095481670928</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01690821256038644</v>
+        <v>0.01161551577152597</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[0.7608695652173914, 0.7777777777777778, 0.7608695652173914, 0.7777777777777778, 0.8222222222222222, 0.7777777777777778, 0.782608695652174, 0.7555555555555555, 0.7608695652173914, 0.7608695652173914]</t>
+          <t>[0.7941176470588235, 0.7941176470588235, 0.8088235294117647, 0.7681159420289855, 0.782608695652174, 0.7971014492753623, 0.7971014492753623, 0.7971014492753623, 0.7971014492753623, 0.7681159420289855]</t>
         </is>
       </c>
     </row>
@@ -875,14 +875,14 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.9096115841539181</v>
+        <v>0.9188537549407114</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02298343322808249</v>
+        <v>0.007185351124969208</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[0.9107328598175279, 0.9084903084903083, 0.8901428472366687, 0.9151624351624352, 0.9252479023646072, 0.9009798984223537, 0.933493961626954, 0.8907516607516608, 0.9377321762905287, 0.8993308369738575]</t>
+          <t>[0.9175669740887132, 0.9236717982647605, 0.9201405357927096, 0.9004040404040403, 0.9269740887132191, 0.915885558768962, 0.911961489141111, 0.9366974088713218, 0.9155535732079393, 0.920272288098375]</t>
         </is>
       </c>
     </row>
@@ -903,14 +903,14 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.7666773456388869</v>
+        <v>0.7908260178336904</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01393346202699774</v>
+        <v>0.008624028907200598</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[0.7629589095612375, 0.7750915750915752, 0.7497105355677954, 0.7708180708180707, 0.8222222222222222, 0.7703957817165363, 0.7842566192276784, 0.759371492704826, 0.762244469870328, 0.7560023338144266]</t>
+          <t>[0.791437908496732, 0.7902141271706489, 0.8080904602643733, 0.7632068697703727, 0.7853782609427278, 0.7984317700304777, 0.7873776786820266, 0.795034164599382, 0.792906083340866, 0.7676355960943275]</t>
         </is>
       </c>
     </row>
@@ -931,14 +931,14 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.7088702147525676</v>
+        <v>0.5914760389839924</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[0.7088702147525676, 0.7088702147525676, 0.7088702147525676, 0.7088702147525676, 0.7088702147525676, 0.7088702147525676, 0.7088702147525676, 0.7088702147525676, 0.7088702147525676, 0.7088702147525676]</t>
+          <t>[0.5914760389839924, 0.5914760389839924, 0.5914760389839924, 0.5914760389839924, 0.5914760389839924, 0.5914760389839924, 0.5914760389839924, 0.5914760389839924, 0.5914760389839924, 0.5914760389839924]</t>
         </is>
       </c>
     </row>
@@ -959,14 +959,14 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.4222222222222222</v>
+        <v>0.4492753623188406</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[0.4222222222222222, 0.4222222222222222, 0.4222222222222222, 0.4222222222222222, 0.4222222222222222, 0.4222222222222222, 0.4222222222222222, 0.4222222222222222, 0.4222222222222222, 0.4222222222222222]</t>
+          <t>[0.4492753623188406, 0.4492753623188406, 0.4492753623188406, 0.4492753623188406, 0.4492753623188406, 0.4492753623188406, 0.4492753623188406, 0.4492753623188406, 0.4492753623188406, 0.4492753623188406]</t>
         </is>
       </c>
     </row>
@@ -1015,14 +1015,14 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.4757201646090535</v>
+        <v>0.4725752508361205</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[0.47572016460905353, 0.47572016460905353, 0.47572016460905353, 0.47572016460905353, 0.47572016460905353, 0.47572016460905353, 0.47572016460905353, 0.47572016460905353, 0.47572016460905353, 0.47572016460905353]</t>
+          <t>[0.47257525083612045, 0.47257525083612045, 0.47257525083612045, 0.47257525083612045, 0.47257525083612045, 0.47257525083612045, 0.47257525083612045, 0.47257525083612045, 0.47257525083612045, 0.47257525083612045]</t>
         </is>
       </c>
     </row>
@@ -1043,14 +1043,14 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.48062558356676</v>
+        <v>0.5190880169671263</v>
       </c>
       <c r="E22" t="n">
-        <v>0.008652448985591144</v>
+        <v>0.01861324239840856</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[0.48062558356676, 0.46908898491930506, 0.48062558356676, 0.48062558356676, 0.5146838345533116, 0.48062558356676, 0.48062558356676, 0.48062558356676, 0.46908898491930506, 0.46908898491930506]</t>
+          <t>[0.5190880169671263, 0.5190880169671263, 0.5190880169671263, 0.5488941069534918, 0.5409958021148839, 0.5190880169671263, 0.5278176311174877, 0.5488941069534918, 0.5190880169671263, 0.5190880169671263]</t>
         </is>
       </c>
     </row>
@@ -1071,14 +1071,14 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.4888888888888889</v>
+        <v>0.5217391304347826</v>
       </c>
       <c r="E23" t="n">
-        <v>0.007971014492753559</v>
+        <v>0.01870204603580561</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[0.4888888888888889, 0.4782608695652174, 0.4888888888888889, 0.4888888888888889, 0.5217391304347826, 0.4888888888888889, 0.4888888888888889, 0.4888888888888889, 0.4782608695652174, 0.4782608695652174]</t>
+          <t>[0.5217391304347826, 0.5217391304347826, 0.5217391304347826, 0.5507246376811594, 0.5441176470588235, 0.5217391304347826, 0.5294117647058824, 0.5507246376811594, 0.5217391304347826, 0.5217391304347826]</t>
         </is>
       </c>
     </row>
@@ -1127,14 +1127,14 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.4826335769731996</v>
+        <v>0.5176662254352917</v>
       </c>
       <c r="E25" t="n">
-        <v>0.009381742607855459</v>
+        <v>0.01814980562395707</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[0.4826335769731996, 0.47012458682939234, 0.4826335769731996, 0.4826335769731996, 0.5142808712602763, 0.4826335769731996, 0.4826335769731996, 0.4826335769731996, 0.47012458682939234, 0.47012458682939234]</t>
+          <t>[0.5176662254352917, 0.5176662254352917, 0.5176662254352917, 0.5468985754089105, 0.5396019733008766, 0.5176662254352917, 0.5244582043343653, 0.5468985754089105, 0.5176662254352917, 0.5176662254352917]</t>
         </is>
       </c>
     </row>
@@ -1155,14 +1155,14 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.6369747899159663</v>
+        <v>0.6324673029338989</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[0.6369747899159663, 0.6369747899159663, 0.6369747899159663, 0.6369747899159663, 0.6369747899159663, 0.6369747899159663, 0.6369747899159663, 0.6369747899159663, 0.6369747899159663, 0.6369747899159663]</t>
+          <t>[0.6324673029338989, 0.6324673029338989, 0.6324673029338989, 0.6324673029338989, 0.6324673029338989, 0.6324673029338989, 0.6324673029338989, 0.6324673029338989, 0.6324673029338989, 0.6324673029338989]</t>
         </is>
       </c>
     </row>
@@ -1183,14 +1183,14 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.4057971014492754</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[0.4666666666666667, 0.4666666666666667, 0.4666666666666667, 0.4666666666666667, 0.4666666666666667, 0.4666666666666667, 0.4666666666666667, 0.4666666666666667, 0.4666666666666667, 0.4666666666666667]</t>
+          <t>[0.4057971014492754, 0.4057971014492754, 0.4057971014492754, 0.4057971014492754, 0.4057971014492754, 0.4057971014492754, 0.4057971014492754, 0.4057971014492754, 0.4057971014492754, 0.4057971014492754]</t>
         </is>
       </c>
     </row>
@@ -1239,14 +1239,14 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.4879999999999999</v>
+        <v>0.4549994444179881</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[0.48799999999999993, 0.48799999999999993, 0.48799999999999993, 0.48799999999999993, 0.48799999999999993, 0.48799999999999993, 0.48799999999999993, 0.48799999999999993, 0.48799999999999993, 0.48799999999999993]</t>
+          <t>[0.4549994444179881, 0.4549994444179881, 0.4549994444179881, 0.4549994444179881, 0.4549994444179881, 0.4549994444179881, 0.4549994444179881, 0.4549994444179881, 0.4549994444179881, 0.4549994444179881]</t>
         </is>
       </c>
     </row>
@@ -1267,14 +1267,14 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.4434343434343434</v>
+        <v>0.3870214752567693</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[0.4434343434343434, 0.4434343434343434, 0.4434343434343434, 0.4434343434343434, 0.4434343434343434, 0.4434343434343434, 0.4434343434343434, 0.4434343434343434, 0.4434343434343434, 0.4434343434343434]</t>
+          <t>[0.38702147525676933, 0.38702147525676933, 0.38702147525676933, 0.38702147525676933, 0.38702147525676933, 0.38702147525676933, 0.38702147525676933, 0.38702147525676933, 0.38702147525676933, 0.38702147525676933]</t>
         </is>
       </c>
     </row>
@@ -1295,14 +1295,14 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.4130434782608696</v>
+        <v>0.3382352941176471</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[0.41304347826086957, 0.41304347826086957, 0.41304347826086957, 0.41304347826086957, 0.41304347826086957, 0.41304347826086957, 0.41304347826086957, 0.41304347826086957, 0.41304347826086957, 0.41304347826086957]</t>
+          <t>[0.3382352941176471, 0.3382352941176471, 0.3382352941176471, 0.3382352941176471, 0.3382352941176471, 0.3382352941176471, 0.3382352941176471, 0.3382352941176471, 0.3382352941176471, 0.3382352941176471]</t>
         </is>
       </c>
     </row>
@@ -1351,14 +1351,14 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.4144590495449949</v>
+        <v>0.3452661210272574</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[0.4144590495449949, 0.4144590495449949, 0.4144590495449949, 0.4144590495449949, 0.4144590495449949, 0.4144590495449949, 0.4144590495449949, 0.4144590495449949, 0.4144590495449949, 0.4144590495449949]</t>
+          <t>[0.3452661210272574, 0.3452661210272574, 0.3452661210272574, 0.3452661210272574, 0.3452661210272574, 0.3452661210272574, 0.3452661210272574, 0.3452661210272574, 0.3452661210272574, 0.3452661210272574]</t>
         </is>
       </c>
     </row>
@@ -1379,14 +1379,14 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.8280709912423467</v>
+        <v>0.8507469782895114</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0248565147784946</v>
+        <v>0.01586049110026089</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[0.8321839080459771, 0.8256606990622337, 0.8256606990622337, 0.8437587657784011, 0.8304812834224597, 0.8107531055900621, 0.8708259061200238, 0.8437587657784011, 0.812791149068323, 0.803864734299517]</t>
+          <t>[0.8402576489533011, 0.8514624505928854, 0.859903381642512, 0.8327294685990339, 0.8529411764705882, 0.8689668174962293, 0.8484364101371774, 0.8874783956135646, 0.8500315059861373, 0.8297125668449198]</t>
         </is>
       </c>
     </row>
@@ -1407,14 +1407,14 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.7913043478260871</v>
+        <v>0.8394075021312872</v>
       </c>
       <c r="E35" t="n">
-        <v>0.02065217391304353</v>
+        <v>0.01449275362318836</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[0.8043478260869565, 0.7608695652173914, 0.8, 0.782608695652174, 0.782608695652174, 0.8, 0.8043478260869565, 0.8222222222222222, 0.7777777777777778, 0.782608695652174]</t>
+          <t>[0.8260869565217391, 0.8260869565217391, 0.8405797101449275, 0.8235294117647058, 0.8529411764705882, 0.8405797101449275, 0.8382352941176471, 0.8695652173913043, 0.8405797101449275, 0.8088235294117647]</t>
         </is>
       </c>
     </row>
@@ -1435,14 +1435,14 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.7755452821242295</v>
+        <v>0.9048335123523092</v>
       </c>
       <c r="E36" t="n">
-        <v>0.05589882645803701</v>
+        <v>0.03892857142857165</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>[0.7635135135135136, 0.7736486486486486, 0.8108108108108109, 0.7601351351351351, 0.7763157894736842, 0.8256578947368421, 0.8614864864864865, 0.8528528528528528, 0.7263513513513513, 0.7747747747747746]</t>
+          <t>[0.9108485499462943, 0.8894736842105263, 0.9231578947368422, 0.9163265306122449, 0.863157894736842, 0.9052631578947368, 0.8705263157894736, 0.9153061224489797, 0.8540816326530613, 0.9044038668098818]</t>
         </is>
       </c>
     </row>
@@ -1463,14 +1463,14 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.8023521528921277</v>
+        <v>0.8427210638056256</v>
       </c>
       <c r="E37" t="n">
-        <v>0.0133863291028864</v>
+        <v>0.01457118920537748</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0.8081564841227548, 0.7851291745431633, 0.8045124899274779, 0.8001918158567775, 0.8001918158567775, 0.8045124899274779, 0.8215184944841012, 0.8296296296296297, 0.7781978575929426, 0.7917482700091397]</t>
+          <t>[0.8302918173408459, 0.8323942477503995, 0.8456530608624696, 0.8235294117647057, 0.8529411764705882, 0.8445952740070386, 0.8418184070357985, 0.873716140705657, 0.8436237205754528, 0.8147992880573084]</t>
         </is>
       </c>
     </row>
@@ -1491,14 +1491,14 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.7466522639301467</v>
+        <v>0.8076651049921575</v>
       </c>
       <c r="E38" t="n">
-        <v>0.04764497486105446</v>
+        <v>0.0352975160751906</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[0.7680335968379446, 0.7188735177865612, 0.7167224080267557, 0.7780100334448161, 0.7503933747412009, 0.7188735177865612, 0.7165013984235952, 0.7619731800766284, 0.7680335968379446, 0.7429111531190926]</t>
+          <t>[0.8132664437012262, 0.8107585139318886, 0.8194065106665682, 0.778149386845039, 0.8235294117647058, 0.7958477508650518, 0.8045716960524263, 0.7564778216952129, 0.8276214833759591, 0.7681159420289855]</t>
         </is>
       </c>
     </row>
@@ -1519,14 +1519,14 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.7282608695652173</v>
+        <v>0.8029624893435635</v>
       </c>
       <c r="E39" t="n">
-        <v>0.03804347826086951</v>
+        <v>0.0369778346121058</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[0.7608695652173914, 0.717391304347826, 0.717391304347826, 0.7608695652173914, 0.7391304347826086, 0.717391304347826, 0.6956521739130435, 0.717391304347826, 0.7608695652173914, 0.7391304347826086]</t>
+          <t>[0.8115942028985508, 0.8088235294117647, 0.8115942028985508, 0.7681159420289855, 0.8235294117647058, 0.7941176470588235, 0.7971014492753623, 0.7536231884057971, 0.8260869565217391, 0.7681159420289855]</t>
         </is>
       </c>
     </row>
@@ -1547,14 +1547,14 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.789</v>
+        <v>0.8692392676767676</v>
       </c>
       <c r="E40" t="n">
-        <v>0.03102380952380945</v>
+        <v>0.01999158249158262</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[0.788, 0.76, 0.7676190476190476, 0.802, 0.8438095238095237, 0.734, 0.7790476190476191, 0.7999999999999999, 0.8457142857142858, 0.79]</t>
+          <t>[0.8577441077441076, 0.8804713804713804, 0.8804713804713805, 0.8493265993265993, 0.8787878787878788, 0.8697916666666666, 0.8484848484848485, 0.8686868686868686, 0.8796296296296297, 0.8644781144781145]</t>
         </is>
       </c>
     </row>
@@ -1575,14 +1575,14 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.7284620622768825</v>
+        <v>0.8020698094604131</v>
       </c>
       <c r="E41" t="n">
-        <v>0.03734176201043893</v>
+        <v>0.03645679215289643</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[0.761208757323466, 0.7177936897711562, 0.7167155303266588, 0.7603042450406005, 0.7391304347826089, 0.7177936897711562, 0.6939229249011858, 0.7177921677459144, 0.761208757323466, 0.7396245059288536]</t>
+          <t>[0.8108764665286405, 0.8069529181535627, 0.8111981427827183, 0.7676263219741482, 0.8235294117647058, 0.7942959001782531, 0.7971867007672634, 0.7537267733591687, 0.8261600292290829, 0.7681159420289855]</t>
         </is>
       </c>
     </row>
@@ -1603,14 +1603,14 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.7902714015662977</v>
+        <v>0.8435054939850336</v>
       </c>
       <c r="E42" t="n">
-        <v>0.009924594733039416</v>
+        <v>0.01131585191961504</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[0.8222826086956523, 0.7655172413793104, 0.7943899018232818, 0.8079999999999999, 0.7907773386034255, 0.7901701323251418, 0.7467720685111989, 0.782608695652174, 0.7903726708074535, 0.7864225781845918]</t>
+          <t>[0.836033634126333, 0.8397058823529412, 0.8067858722436343, 0.847305105617126, 0.8272946859903381, 0.8622052610058607, 0.8683049779458096, 0.847305105617126, 0.8369565217391305, 0.8476719087264878]</t>
         </is>
       </c>
     </row>
@@ -1631,14 +1631,14 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.7582125603864734</v>
+        <v>0.8175618073316283</v>
       </c>
       <c r="E43" t="n">
-        <v>0.038768115942029</v>
+        <v>0.02605498721227628</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[0.7777777777777778, 0.7333333333333333, 0.782608695652174, 0.7333333333333333, 0.7391304347826086, 0.7608695652173914, 0.7111111111111111, 0.7555555555555555, 0.7608695652173914, 0.7777777777777778]</t>
+          <t>[0.8260869565217391, 0.8088235294117647, 0.7681159420289855, 0.8382352941176471, 0.7971014492753623, 0.8405797101449275, 0.8115942028985508, 0.8260869565217391, 0.7971014492753623, 0.8235294117647058]</t>
         </is>
       </c>
     </row>
@@ -1659,14 +1659,14 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.8158508158508159</v>
+        <v>0.8357142857142856</v>
       </c>
       <c r="E44" t="n">
-        <v>0.02376565428036026</v>
+        <v>0.03469030969030973</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[0.8181818181818181, 0.76010101010101, 0.8333333333333333, 0.8207070707070707, 0.797979797979798, 0.8434343434343434, 0.8063725490196078, 0.8065268065268066, 0.8391608391608392, 0.8135198135198136]</t>
+          <t>[0.8064935064935065, 0.8671328671328671, 0.7496503496503497, 0.8337662337662337, 0.8311688311688311, 0.7958041958041958, 0.8475524475524476, 0.855944055944056, 0.8376623376623377, 0.8467532467532468]</t>
         </is>
       </c>
     </row>
@@ -1687,14 +1687,14 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.7633870691841707</v>
+        <v>0.8248217577685051</v>
       </c>
       <c r="E45" t="n">
-        <v>0.03152292030072823</v>
+        <v>0.02493358075777408</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[0.7888888888888889, 0.743778801843318, 0.7869759316770187, 0.7482758620689655, 0.7443711180124224, 0.7741475639758122, 0.7202821869488537, 0.76331569664903, 0.7634584417193113, 0.7777777777777778]</t>
+          <t>[0.8302737520128824, 0.8196891659889761, 0.779977375565611, 0.8336751435602954, 0.8039585645578986, 0.8511045448149712, 0.8261141037723043, 0.8336751435602954, 0.7995642701525054, 0.8235294117647058]</t>
         </is>
       </c>
     </row>
@@ -1715,14 +1715,14 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.6714021164021164</v>
+        <v>0.7562257009827342</v>
       </c>
       <c r="E46" t="n">
-        <v>0.02949877449019322</v>
+        <v>0.01778871631044388</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[0.6750658761528328, 0.6395881006864989, 0.6222222222222222, 0.6617715617715618, 0.6276742581090408, 0.6733333333333333, 0.6975468975468976, 0.6721693121693122, 0.6706349206349206, 0.6773590859268609]</t>
+          <t>[0.7258855154965211, 0.7476190476190475, 0.7570419918246006, 0.7554094101408679, 0.7688917574501098, 0.7706368194776743, 0.7655228758169935, 0.747132514618337, 0.7659169550173011, 0.7492617327699785]</t>
         </is>
       </c>
     </row>
@@ -1743,14 +1743,14 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.6483091787439614</v>
+        <v>0.7391304347826086</v>
       </c>
       <c r="E47" t="n">
-        <v>0.02995169082125604</v>
+        <v>0.0244565217391306</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[0.6521739130434783, 0.6086956521739131, 0.6222222222222222, 0.6444444444444445, 0.6222222222222222, 0.6521739130434783, 0.6888888888888889, 0.6222222222222222, 0.6521739130434783, 0.6739130434782609]</t>
+          <t>[0.7058823529411765, 0.7246376811594203, 0.7536231884057971, 0.7391304347826086, 0.7536231884057971, 0.7391304347826086, 0.7647058823529411, 0.7391304347826086, 0.75, 0.7205882352941176]</t>
         </is>
       </c>
     </row>
@@ -1771,14 +1771,14 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.7753738393124583</v>
+        <v>0.8616160166306313</v>
       </c>
       <c r="E48" t="n">
-        <v>0.01611738540665719</v>
+        <v>0.01385608788970127</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[0.7740736717718816, 0.7692650598829087, 0.7383283283283283, 0.783729472987785, 0.763945763945764, 0.776674006853035, 0.7777386477386478, 0.7866812266812265, 0.765064155064155, 0.7919032477856006]</t>
+          <t>[0.8605026200203402, 0.8802459376372419, 0.8622749231444884, 0.860957110116774, 0.8767149758454106, 0.8546332894158981, 0.8470267896354852, 0.8822469699342188, 0.8639375117635987, 0.859385155906895]</t>
         </is>
       </c>
     </row>
@@ -1799,14 +1799,14 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.647077204810758</v>
+        <v>0.7439365559779477</v>
       </c>
       <c r="E49" t="n">
-        <v>0.03292229630219745</v>
+        <v>0.02288243958210445</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[0.6557153753950091, 0.6136206788380701, 0.6197802197802198, 0.6499900183871816, 0.6238495398159264, 0.6597101449275362, 0.6871822582460881, 0.631608005521049, 0.6441643912343344, 0.6699660807893926]</t>
+          <t>[0.7116510372264847, 0.7264282916456828, 0.7536364998627019, 0.7412343252132799, 0.7518360752056404, 0.7466387867426155, 0.764117695041473, 0.7403640024938072, 0.753114186851211, 0.7225816837176445]</t>
         </is>
       </c>
     </row>
@@ -1827,14 +1827,14 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.786163759962387</v>
+        <v>0.8397251656100464</v>
       </c>
       <c r="E50" t="n">
-        <v>0.02962128947490106</v>
+        <v>0.01976642473812851</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[0.7741452991452991, 0.7821019560149994, 0.7669226830517153, 0.8047685834502104, 0.8362318840579711, 0.7993650793650795, 0.7658719027582982, 0.8215488215488216, 0.7736801242236025, 0.7902255639097746]</t>
+          <t>[0.8484364101371774, 0.8514624505928854, 0.859903381642512, 0.8359150326797385, 0.816092401026678, 0.8302044221944096, 0.8331447963800905, 0.8435352985403541, 0.8718081435472739, 0.8219911783238816]</t>
         </is>
       </c>
     </row>
@@ -1855,14 +1855,14 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.7391304347826086</v>
+        <v>0.8321611253196931</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0204106280193237</v>
+        <v>0.0266410912190963</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[0.7608695652173914, 0.7391304347826086, 0.7391304347826086, 0.7391304347826086, 0.7391304347826086, 0.7391304347826086, 0.717391304347826, 0.7777777777777778, 0.7555555555555555, 0.782608695652174]</t>
+          <t>[0.8382352941176471, 0.8260869565217391, 0.8405797101449275, 0.8382352941176471, 0.8115942028985508, 0.8115942028985508, 0.8382352941176471, 0.8115942028985508, 0.8695652173913043, 0.7971014492753623]</t>
         </is>
       </c>
     </row>
@@ -1883,14 +1883,14 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.6699512012012012</v>
+        <v>0.8438775510204082</v>
       </c>
       <c r="E52" t="n">
-        <v>0.03464566540224434</v>
+        <v>0.006241944146079481</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>[0.652027027027027, 0.6726726726726727, 0.6201201201201201, 0.6921921921921922, 0.7565789473684211, 0.6672297297297297, 0.6611842105263158, 0.6973684210526315, 0.6621621621621623, 0.7088815789473684]</t>
+          <t>[0.8039742212674543, 0.8700322234156821, 0.85, 0.8438775510204082, 0.8438775510204082, 0.8489473684210527, 0.8438775510204082, 0.8399999999999999, 0.8610526315789474, 0.8433673469387755]</t>
         </is>
       </c>
     </row>
@@ -1911,14 +1911,14 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.7618768060583917</v>
+        <v>0.8311825634257147</v>
       </c>
       <c r="E53" t="n">
-        <v>0.01369489555983827</v>
+        <v>0.02394650488755357</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[0.7655245917055893, 0.7553924336533031, 0.7500979240109673, 0.760230179028133, 0.7672634271099745, 0.7635234330886504, 0.7238192668371696, 0.7936507936507935, 0.7523809523809523, 0.782608695652174]</t>
+          <t>[0.8415993354979989, 0.8286601597160603, 0.8456530608624696, 0.8368662780427487, 0.8130581174059436, 0.8155736062067029, 0.8337049671353691, 0.8191574463664225, 0.8704835412316471, 0.8059231253938248]</t>
         </is>
       </c>
     </row>
@@ -1939,14 +1939,14 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.8079697476436607</v>
+        <v>0.8074091742007785</v>
       </c>
       <c r="E54" t="n">
-        <v>0.02658543137431457</v>
+        <v>0.02988316918943523</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>[0.822742474916388, 0.804180602006689, 0.7928743961352657, 0.7988779803646564, 0.8554841897233202, 0.7945341614906832, 0.8015873015873015, 0.8117588932806324, 0.827273497754047, 0.8298676748582231]</t>
+          <t>[0.780035650623886, 0.7905354449472097, 0.7941176470588235, 0.8001499250374813, 0.8146684233640756, 0.8276214833759591, 0.8313748531139835, 0.8146684233640756, 0.8235294117647058, 0.783729209841118]</t>
         </is>
       </c>
     </row>
@@ -1967,14 +1967,14 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.8043478260869565</v>
+        <v>0.8029624893435635</v>
       </c>
       <c r="E55" t="n">
-        <v>0.01739130434782599</v>
+        <v>0.03436700767263423</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[0.8043478260869565, 0.8043478260869565, 0.7777777777777778, 0.782608695652174, 0.8478260869565217, 0.782608695652174, 0.8, 0.8043478260869565, 0.8043478260869565, 0.8260869565217391]</t>
+          <t>[0.7794117647058824, 0.782608695652174, 0.7941176470588235, 0.7971014492753623, 0.8088235294117647, 0.8260869565217391, 0.8260869565217391, 0.8088235294117647, 0.8235294117647058, 0.782608695652174]</t>
         </is>
       </c>
     </row>
@@ -1995,14 +1995,14 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.8352380952380952</v>
+        <v>0.8253607503607503</v>
       </c>
       <c r="E56" t="n">
-        <v>0.01555952380952386</v>
+        <v>0.04773647937710424</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[0.8352380952380952, 0.8580952380952381, 0.838, 0.8304761904761906, 0.8559999999999999, 0.8161904761904761, 0.8150000000000001, 0.8247619047619048, 0.843, 0.8352380952380952]</t>
+          <t>[0.7710437710437711, 0.7899831649831649, 0.8428819444444444, 0.8350649350649352, 0.8585858585858586, 0.8484848484848484, 0.8156565656565655, 0.811026936026936, 0.8535353535353535, 0.7954545454545455]</t>
         </is>
       </c>
     </row>
@@ -2023,14 +2023,14 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.803138893476945</v>
+        <v>0.8010340810982034</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0168292176417959</v>
+        <v>0.03414311497876077</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[0.8038852913968547, 0.8038799825338406, 0.7777777777777778, 0.7813545150501673, 0.8474663377531092, 0.782608695652174, 0.8003982080637134, 0.8038852913968547, 0.8023978044200493, 0.8264163372859025]</t>
+          <t>[0.7795551590083487, 0.7827000941404428, 0.7941176470588235, 0.7958957702812431, 0.8061723919151637, 0.8261600292290829, 0.8259408111070515, 0.8082021541010771, 0.8235294117647058, 0.7827000941404428]</t>
         </is>
       </c>
     </row>
@@ -2051,14 +2051,14 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.8241847826086957</v>
+        <v>0.8365935504636637</v>
       </c>
       <c r="E58" t="n">
-        <v>0.01980801806888766</v>
+        <v>0.02427463692649112</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[0.82, 0.8443817052512704, 0.8093944099378882, 0.8622222222222221, 0.82, 0.8260869565217391, 0.8260869565217391, 0.82, 0.8764976958525345, 0.8222826086956523]</t>
+          <t>[0.8334812185743863, 0.8167471819645733, 0.8266402714932126, 0.84317615935263, 0.8397058823529412, 0.8260869565217391, 0.861916264090177, 0.8135011441647597, 0.8692455242966752, 0.8529411764705882]</t>
         </is>
       </c>
     </row>
@@ -2079,14 +2079,14 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.8043478260869565</v>
+        <v>0.8115942028985508</v>
       </c>
       <c r="E59" t="n">
-        <v>0.01630434782608692</v>
+        <v>0.002078005115089487</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[0.8043478260869565, 0.8043478260869565, 0.8043478260869565, 0.8444444444444444, 0.8, 0.8043478260869565, 0.8260869565217391, 0.8, 0.8666666666666667, 0.8043478260869565]</t>
+          <t>[0.8088235294117647, 0.8115942028985508, 0.8088235294117647, 0.8115942028985508, 0.8115942028985508, 0.8115942028985508, 0.8405797101449275, 0.8115942028985508, 0.8088235294117647, 0.8260869565217391]</t>
         </is>
       </c>
     </row>
@@ -2107,14 +2107,14 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.8362470862470863</v>
+        <v>0.7622377622377623</v>
       </c>
       <c r="E60" t="n">
-        <v>0.01084230312171497</v>
+        <v>0.02729770229770234</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>[0.7979797979797979, 0.8356643356643357, 0.8345588235294117, 0.8473193473193473, 0.8396464646464646, 0.8611111111111112, 0.8368298368298368, 0.775735294117647, 0.8876262626262627, 0.8345588235294118]</t>
+          <t>[0.7524475524475525, 0.7209790209790209, 0.7643356643356644, 0.7601398601398601, 0.7839160839160839, 0.7475524475524475, 0.8146853146853147, 0.7558441558441559, 0.8474025974025974, 0.7706293706293705]</t>
         </is>
       </c>
     </row>
@@ -2135,14 +2135,14 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.8081376893970598</v>
+        <v>0.8170506666190216</v>
       </c>
       <c r="E61" t="n">
-        <v>0.0165598955208387</v>
+        <v>0.009517847768461096</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[0.8063492063492064, 0.8134923293361025, 0.8064659977703456, 0.8493827160493829, 0.8063492063492064, 0.8064659977703456, 0.8260869565217391, 0.8063492063492064, 0.8697115384615384, 0.809809381023774]</t>
+          <t>[0.8160319235654301, 0.8139783319349498, 0.8160319235654301, 0.8139783319349498, 0.8213815170336908, 0.8180694096726132, 0.8528657801150268, 0.80279081698089, 0.8248855978034778, 0.8260869565217391]</t>
         </is>
       </c>
     </row>
@@ -2163,14 +2163,14 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.7445746794163618</v>
+        <v>0.7089031758948638</v>
       </c>
       <c r="E62" t="n">
-        <v>0.04461766045603544</v>
+        <v>0.01228955734728554</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>[0.7598600080764571, 0.7907716102423098, 0.723731884057971, 0.7473838779368079, 0.7848765432098765, 0.7122873345935727, 0.7229249011857708, 0.7417654808959157, 0.7244444444444444, 0.7714169101220141]</t>
+          <t>[0.7034313725490196, 0.7371587850826604, 0.7059366038905681, 0.6821552150271873, 0.701981913455037, 0.6944444444444444, 0.7419772256728778, 0.7132139812446718, 0.715107120352867, 0.7118697478991597]</t>
         </is>
       </c>
     </row>
@@ -2191,14 +2191,14 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.7173913043478261</v>
+        <v>0.6764705882352942</v>
       </c>
       <c r="E63" t="n">
-        <v>0.03417874396135268</v>
+        <v>0.02541560102301776</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>[0.717391304347826, 0.7608695652173914, 0.7111111111111111, 0.7391304347826086, 0.717391304347826, 0.6956521739130435, 0.717391304347826, 0.6888888888888889, 0.6956521739130435, 0.7391304347826086]</t>
+          <t>[0.6617647058823529, 0.6956521739130435, 0.6956521739130435, 0.6764705882352942, 0.6764705882352942, 0.6666666666666666, 0.6956521739130435, 0.6911764705882353, 0.6764705882352942, 0.6617647058823529]</t>
         </is>
       </c>
     </row>
@@ -2219,14 +2219,14 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.7951078281169814</v>
+        <v>0.8074174154592668</v>
       </c>
       <c r="E64" t="n">
-        <v>0.03153451227535886</v>
+        <v>0.01351187127518994</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[0.8196256451405192, 0.8092080497686905, 0.7605519155519157, 0.802434693453, 0.8144485394485395, 0.7505101687023883, 0.7877809627809629, 0.7863085813085813, 0.775981455615323, 0.8103943158290984]</t>
+          <t>[0.7937812911725955, 0.8448484848484848, 0.8148792270531401, 0.8096448856222331, 0.8005709266578832, 0.8143745566408382, 0.7846296757339299, 0.8051899452963004, 0.8216136738786423, 0.8032519727258491]</t>
         </is>
       </c>
     </row>
@@ -2247,14 +2247,14 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.7192126049129798</v>
+        <v>0.6844102749650594</v>
       </c>
       <c r="E65" t="n">
-        <v>0.03037953795162129</v>
+        <v>0.01909406394607094</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[0.7144366804692892, 0.7692028985507247, 0.7226270805218173, 0.740011244377811, 0.7228051571133559, 0.7022946859903382, 0.7157981293041422, 0.6858418702390333, 0.6922855707696024, 0.7522482837528603]</t>
+          <t>[0.6663865546218487, 0.6959853406630019, 0.6953391196541061, 0.6785714285714285, 0.6814769020309377, 0.6671341748480598, 0.6958944770039223, 0.6965877259994908, 0.687343647899181, 0.6760249554367203]</t>
         </is>
       </c>
     </row>
@@ -2275,14 +2275,14 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.8564102564102565</v>
+        <v>0.867672608721202</v>
       </c>
       <c r="E66" t="n">
-        <v>0.002600195256610927</v>
+        <v>0.008094898768657099</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[0.8564102564102565, 0.8361801242236023, 0.8570048309178743, 0.8267610380856084, 0.8552845528455284, 0.8564102564102565, 0.8581780538302277, 0.8845410628019322, 0.8616021659499921, 0.8552845528455284]</t>
+          <t>[0.8684359119141727, 0.8762541806020068, 0.8669093055282313, 0.8817299495048856, 0.869296833064949, 0.8644654977375565, 0.8520412996116321, 0.8663351107465136, 0.8972719522591646, 0.8666744475568005]</t>
         </is>
       </c>
     </row>
@@ -2303,14 +2303,14 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="E67" t="n">
-        <v>0.01630434782608692</v>
+        <v>0.001918158567774886</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[0.8666666666666667, 0.8478260869565217, 0.8478260869565217, 0.8478260869565217, 0.8666666666666667, 0.8666666666666667, 0.8695652173913043, 0.8695652173913043, 0.8695652173913043, 0.8666666666666667]</t>
+          <t>[0.8695652173913043, 0.8695652173913043, 0.8405797101449275, 0.8840579710144928, 0.8695652173913043, 0.8676470588235294, 0.855072463768116, 0.8695652173913043, 0.8840579710144928, 0.8676470588235294]</t>
         </is>
       </c>
     </row>
@@ -2331,14 +2331,14 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.8433499288762447</v>
+        <v>0.9314070891514501</v>
       </c>
       <c r="E68" t="n">
-        <v>0.04391891891891897</v>
+        <v>0.01349892588614399</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[0.8421052631578948, 0.8344594594594594, 0.8783783783783784, 0.8209459459459459, 0.8682432432432433, 0.8445945945945946, 0.9155405405405406, 0.8716216216216216, 0.8243243243243243, 0.8209459459459459]</t>
+          <t>[0.9494736842105262, 0.9410526315789474, 0.9368421052631579, 0.9301825993555317, 0.9294736842105263, 0.9221052631578948, 0.9255102040816325, 0.9326315789473685, 0.9129967776584318, 0.9463157894736841]</t>
         </is>
       </c>
     </row>
@@ -2359,14 +2359,14 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.8427947957839261</v>
+        <v>0.8631018622576243</v>
       </c>
       <c r="E69" t="n">
-        <v>0.01099620120365075</v>
+        <v>0.005123643866882244</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[0.8418478260869564, 0.8233775030693028, 0.843741765480896, 0.8222222222222222, 0.8478632478632478, 0.8418478260869564, 0.851086956521739, 0.8671525380386138, 0.8352067868504772, 0.8478632478632478]</t>
+          <t>[0.8627893845285151, 0.8600790513833992, 0.8469793776946652, 0.8819740456569101, 0.8634143399867334, 0.863940427656211, 0.8527078565980168, 0.865874690948562, 0.8739403882964178, 0.8608327708841701]</t>
         </is>
       </c>
     </row>
@@ -2387,14 +2387,14 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.8189229249011858</v>
+        <v>0.8243704437930894</v>
       </c>
       <c r="E70" t="n">
-        <v>0.0187188161444457</v>
+        <v>0.02054767094294663</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[0.8260869565217391, 0.8111111111111111, 0.7780100334448161, 0.827273497754047, 0.8479096989966556, 0.8117588932806324, 0.8479096989966556, 0.8074534161490682, 0.826526130873957, 0.7882529323573506]</t>
+          <t>[0.8546712802768166, 0.8252595155709341, 0.8264617691154422, 0.8356037151702786, 0.8313748531139835, 0.8116186839012927, 0.8001499250374813, 0.8089256535947712, 0.8234813720152446, 0.8087594235601825]</t>
         </is>
       </c>
     </row>
@@ -2415,14 +2415,14 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.8132850241545894</v>
+        <v>0.8115942028985508</v>
       </c>
       <c r="E71" t="n">
-        <v>0.02499999999999991</v>
+        <v>0.01593137254901955</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>[0.8260869565217391, 0.8, 0.7608695652173914, 0.8260869565217391, 0.8478260869565217, 0.8043478260869565, 0.8478260869565217, 0.8043478260869565, 0.8222222222222222, 0.782608695652174]</t>
+          <t>[0.8529411764705882, 0.8235294117647058, 0.8115942028985508, 0.8260869565217391, 0.8260869565217391, 0.8115942028985508, 0.7971014492753623, 0.8088235294117647, 0.8115942028985508, 0.8088235294117647]</t>
         </is>
       </c>
     </row>
@@ -2443,14 +2443,14 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.905</v>
+        <v>0.912037037037037</v>
       </c>
       <c r="E72" t="n">
-        <v>0.01500000000000001</v>
+        <v>0.008947924182299172</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>[0.902, 0.8971428571428572, 0.8838095238095238, 0.908, 0.9, 0.9295238095238095, 0.916, 0.9295238095238096, 0.9119999999999999, 0.9]</t>
+          <t>[0.9021645021645022, 0.9132996632996633, 0.9056277056277056, 0.9318181818181819, 0.9124579124579124, 0.9217171717171717, 0.9116161616161617, 0.898989898989899, 0.9124579124579124, 0.9036458333333333]</t>
         </is>
       </c>
     </row>
@@ -2471,14 +2471,14 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.8136883348261701</v>
+        <v>0.810958904109589</v>
       </c>
       <c r="E73" t="n">
-        <v>0.02481891592249519</v>
+        <v>0.01599507729069161</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[0.8260869565217391, 0.8, 0.7612100451909782, 0.8233748622764641, 0.8474622086374317, 0.8046253469010175, 0.8474622086374317, 0.8023600681517005, 0.8227513227513227, 0.7813545150501673]</t>
+          <t>[0.8530685001273236, 0.8236822001527884, 0.8104824300178677, 0.8250535173839226, 0.8259408111070515, 0.8114353782013104, 0.7958957702812431, 0.8086992543496273, 0.8087646800929079, 0.8086156837164089]</t>
         </is>
       </c>
     </row>
@@ -2499,14 +2499,14 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.8555241859589686</v>
+        <v>0.8843293839274839</v>
       </c>
       <c r="E74" t="n">
-        <v>0.02350176263219739</v>
+        <v>0.01522632493942133</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>[0.8716666666666666, 0.843840579710145, 0.8888888888888888, 0.8666666666666667, 0.8666666666666667, 0.843840579710145, 0.8443817052512704, 0.8388888888888889, 0.8180778032036613, 0.8675675675675676]</t>
+          <t>[0.8920385395537526, 0.8944327731092437, 0.8793541825578438, 0.8783591255219849, 0.8637544435329505, 0.8823529411764706, 0.8863058266784974, 0.8640581232492996, 0.8944327731092437, 0.9191960623461854]</t>
         </is>
       </c>
     </row>
@@ -2527,14 +2527,14 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.8572463768115942</v>
+        <v>0.8832054560954816</v>
       </c>
       <c r="E75" t="n">
-        <v>0.01884057971014497</v>
+        <v>0.02429667519181589</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[0.8695652173913043, 0.8478260869565217, 0.8695652173913043, 0.8666666666666667, 0.8666666666666667, 0.8478260869565217, 0.8478260869565217, 0.8444444444444444, 0.8260869565217391, 0.8666666666666667]</t>
+          <t>[0.8970588235294118, 0.8970588235294118, 0.8823529411764706, 0.8840579710144928, 0.8695652173913043, 0.8823529411764706, 0.8695652173913043, 0.8676470588235294, 0.8970588235294118, 0.9130434782608695]</t>
         </is>
       </c>
     </row>
@@ -2555,14 +2555,14 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.9055858357328945</v>
+        <v>0.8844155844155844</v>
       </c>
       <c r="E76" t="n">
-        <v>0.03761312217194579</v>
+        <v>0.04383116883116889</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[0.9277389277389277, 0.8712121212121212, 0.9067599067599067, 0.9207459207459208, 0.9184149184149184, 0.9068627450980393, 0.8904428904428905, 0.8737373737373737, 0.9044117647058824, 0.8686868686868686]</t>
+          <t>[0.8657342657342657, 0.9174825174825176, 0.8993006993006993, 0.8545454545454545, 0.8883116883116884, 0.8805194805194805, 0.9342657342657343, 0.8571428571428572, 0.8792207792207792, 0.9230769230769231]</t>
         </is>
       </c>
     </row>
@@ -2583,14 +2583,14 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.8505277252678008</v>
+        <v>0.8804271708683473</v>
       </c>
       <c r="E77" t="n">
-        <v>0.01889808928011116</v>
+        <v>0.02572534657243808</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[0.8660485933503835, 0.8412098298676749, 0.8554347826086957, 0.8614342179559572, 0.8666666666666667, 0.8422236642872594, 0.845620667926906, 0.8367149758454108, 0.8135265700483091, 0.8571428571428571]</t>
+          <t>[0.8897290485192186, 0.8954636989931107, 0.8785014005602241, 0.8764302059496567, 0.8634705656021547, 0.8823529411764706, 0.8636795855465931, 0.8655961844197139, 0.8954636989931107, 0.9151368760064412]</t>
         </is>
       </c>
     </row>
@@ -2611,14 +2611,14 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.7432017660278529</v>
+        <v>0.7764722167936942</v>
       </c>
       <c r="E78" t="n">
-        <v>0.02872401324433471</v>
+        <v>0.03057595709830996</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[0.7440754897276637, 0.7316549235263791, 0.695715925028688, 0.7318783068783067, 0.7748473748473749, 0.7166416791604198, 0.7824534161490684, 0.7490118577075099, 0.7642424242424243, 0.7423280423280423]</t>
+          <t>[0.739108801415303, 0.8067318644200935, 0.7943452922964851, 0.7826363103380887, 0.7458127415726017, 0.7604433077578857, 0.7828689370485036, 0.7622710622710622, 0.7955661170764146, 0.7703081232492996]</t>
         </is>
       </c>
     </row>
@@ -2639,14 +2639,14 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.7362318840579709</v>
+        <v>0.7720588235294117</v>
       </c>
       <c r="E79" t="n">
-        <v>0.01811594202898548</v>
+        <v>0.04033461210571188</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[0.7391304347826086, 0.717391304347826, 0.717391304347826, 0.7333333333333333, 0.7777777777777778, 0.7391304347826086, 0.782608695652174, 0.7333333333333333, 0.7555555555555555, 0.7333333333333333]</t>
+          <t>[0.7391304347826086, 0.7971014492753623, 0.7941176470588235, 0.782608695652174, 0.7391304347826086, 0.7536231884057971, 0.7794117647058824, 0.75, 0.7971014492753623, 0.7647058823529411]</t>
         </is>
       </c>
     </row>
@@ -2667,14 +2667,14 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.8781709783863505</v>
+        <v>0.9030562580763531</v>
       </c>
       <c r="E80" t="n">
-        <v>0.02459632631829423</v>
+        <v>0.01180278476673935</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>[0.8847261583834474, 0.8649267449267449, 0.8506592568377463, 0.8873664573664573, 0.8915866741953699, 0.8522960300453907, 0.9150395752226416, 0.8716157983892537, 0.8687157617363567, 0.8915049481411037]</t>
+          <t>[0.9035565214227984, 0.917777508730765, 0.9025559947299079, 0.8964239673141984, 0.8969894207683073, 0.8999560825647783, 0.8985468050856708, 0.9143346508563901, 0.9037180089427075, 0.9130298759820135]</t>
         </is>
       </c>
     </row>
@@ -2695,14 +2695,14 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.7311641268784126</v>
+        <v>0.7683947067178469</v>
       </c>
       <c r="E81" t="n">
-        <v>0.01266664523652095</v>
+        <v>0.03928376777481624</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[0.7362762496302868, 0.7228260869565217, 0.6928053830227744, 0.7307820222105936, 0.775599128540305, 0.7181964573268921, 0.7790202366277259, 0.7315462315462316, 0.7362420188507145, 0.7259259259259259]</t>
+          <t>[0.7296599471895705, 0.7966622749231445, 0.7932344108814696, 0.7800741918388977, 0.7364980688963859, 0.7523444160272805, 0.7768387758379975, 0.7500993124522537, 0.795665230447839, 0.7599506375976963]</t>
         </is>
       </c>
     </row>
@@ -2723,14 +2723,14 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.8579152731326645</v>
+        <v>0.8549958596428129</v>
       </c>
       <c r="E82" t="n">
-        <v>0.01668133033456487</v>
+        <v>0.0245900662315387</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>[0.8407389711737537, 0.8361801242236023, 0.8564102564102565, 0.8097826086956522, 0.8822222222222222, 0.8594202898550726, 0.8616021659499921, 0.8552845528455284, 0.8594202898550726, 0.8627783669141039]</t>
+          <t>[0.8355919442875965, 0.8762541806020068, 0.8333722377840025, 0.8605107504274943, 0.8387610116510372, 0.8625232838126391, 0.8494809688581315, 0.8644654977375565, 0.8412764771460424, 0.872005323868678]</t>
         </is>
       </c>
     </row>
@@ -2751,14 +2751,14 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.854006820119352</v>
       </c>
       <c r="E83" t="n">
-        <v>0.02427536231884064</v>
+        <v>0.02392369991474852</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[0.8478260869565217, 0.8444444444444444, 0.8260869565217391, 0.8260869565217391, 0.8888888888888888, 0.8695652173913043, 0.8695652173913043, 0.8666666666666667, 0.8695652173913043, 0.8666666666666667]</t>
+          <t>[0.8405797101449275, 0.8695652173913043, 0.8382352941176471, 0.855072463768116, 0.8405797101449275, 0.855072463768116, 0.8529411764705882, 0.8676470588235294, 0.8405797101449275, 0.8695652173913043]</t>
         </is>
       </c>
     </row>
@@ -2779,14 +2779,14 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.8526997392128971</v>
+        <v>0.9093984962406014</v>
       </c>
       <c r="E84" t="n">
-        <v>0.03551742532005686</v>
+        <v>0.01537593984962415</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>[0.8388157894736842, 0.8468468468468469, 0.9155405405405406, 0.8412162162162161, 0.8648648648648649, 0.8585526315789473, 0.9290540540540541, 0.8782894736842105, 0.8288288288288289, 0.8092105263157895]</t>
+          <t>[0.9347368421052631, 0.9042105263157895, 0.9226638023630505, 0.8852631578947368, 0.9021052631578947, 0.9063157894736842, 0.9122448979591836, 0.9172932330827068, 0.9065520945220193, 0.9210526315789473]</t>
         </is>
       </c>
     </row>
@@ -2807,14 +2807,14 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.8510697032436163</v>
+        <v>0.8457216380916295</v>
       </c>
       <c r="E85" t="n">
-        <v>0.0314200292461162</v>
+        <v>0.02780887140780841</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[0.843741765480896, 0.8233775030693028, 0.8260869565217391, 0.8158942506768594, 0.8782328782328783, 0.8619206880076445, 0.863129290617849, 0.8478632478632478, 0.8619206880076445, 0.8542761586239848]</t>
+          <t>[0.8322981366459627, 0.8686616597471659, 0.8299067199695415, 0.8570134575569358, 0.8364843534882278, 0.8411164787976382, 0.8503267973856209, 0.863940427656211, 0.8337049671353691, 0.8705786966656531]</t>
         </is>
       </c>
     </row>
@@ -2835,14 +2835,14 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.8554841897233202</v>
+        <v>0.8479202066690505</v>
       </c>
       <c r="E86" t="n">
-        <v>0.01808704897949753</v>
+        <v>0.01331415895498889</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>[0.8479096989966556, 0.8733459357277884, 0.871429782184931, 0.8528765920070267, 0.8554841897233202, 0.898550724637681, 0.8554841897233202, 0.8386749482401656, 0.8695652173913043, 0.8528765920070267]</t>
+          <t>[0.8529411764705882, 0.8574140531544183, 0.8382481152879635, 0.8529411764705882, 0.8728590250329381, 0.8437637241985068, 0.8488226175537019, 0.8021445358401881, 0.8470177957843992, 0.826890756302521]</t>
         </is>
       </c>
     </row>
@@ -2863,14 +2863,14 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.8478260869565217</v>
+        <v>0.8405797101449275</v>
       </c>
       <c r="E87" t="n">
-        <v>0.02173913043478259</v>
+        <v>0.01470588235294112</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>[0.8478260869565217, 0.8695652173913043, 0.8695652173913043, 0.8444444444444444, 0.8478260869565217, 0.8695652173913043, 0.8478260869565217, 0.8260869565217391, 0.8695652173913043, 0.8478260869565217]</t>
+          <t>[0.8529411764705882, 0.8529411764705882, 0.8382352941176471, 0.8529411764705882, 0.8695652173913043, 0.8405797101449275, 0.8405797101449275, 0.7971014492753623, 0.8382352941176471, 0.8235294117647058]</t>
         </is>
       </c>
     </row>
@@ -2891,14 +2891,14 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.9326666666666666</v>
+        <v>0.916017316017316</v>
       </c>
       <c r="E88" t="n">
-        <v>0.02049999999999985</v>
+        <v>0.01832123316498313</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[0.9119999999999999, 0.932, 0.916, 0.9139999999999999, 0.9409523809523809, 0.9428571428571428, 0.937142857142857, 0.9333333333333332, 0.9504761904761905, 0.93]</t>
+          <t>[0.8998316498316499, 0.9184027777777777, 0.9292929292929293, 0.9259259259259259, 0.9309764309764309, 0.9132996632996633, 0.9031986531986532, 0.9142857142857141, 0.8973063973063973, 0.9177489177489178]</t>
         </is>
       </c>
     </row>
@@ -2919,14 +2919,14 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.8480423462545958</v>
+        <v>0.8406132229239596</v>
       </c>
       <c r="E89" t="n">
-        <v>0.02121411966376174</v>
+        <v>0.01468920597908019</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[0.8474622086374317, 0.8695652173913043, 0.8688127090301003, 0.8449062620264997, 0.8480419364785693, 0.8688241106719368, 0.8480419364785693, 0.8260869565217391, 0.8695652173913043, 0.8480427560306225]</t>
+          <t>[0.8529411764705882, 0.8521719062516027, 0.8380594246831153, 0.8529411764705882, 0.8695652173913043, 0.8405797101449275, 0.8406467357029915, 0.7969309462915601, 0.8380603376977007, 0.8222910216718267]</t>
         </is>
       </c>
     </row>
@@ -2947,14 +2947,14 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.8681159420289855</v>
+        <v>0.8944132426720177</v>
       </c>
       <c r="E90" t="n">
-        <v>0.02314795095199584</v>
+        <v>0.01546253455082935</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[0.8525387655822437, 0.8695652173913043, 0.8764976958525345, 0.8695652173913043, 0.8716542629586108, 0.8666666666666667, 0.8449488491048593, 0.870137299771167, 0.8208643426034731, 0.8378151260504202]</t>
+          <t>[0.8952205882352942, 0.8783591255219849, 0.8831670230458541, 0.8783591255219849, 0.8663999044433828, 0.9084810957875973, 0.8944327731092437, 0.8944327731092437, 0.8943937122347917, 0.8952205882352942]</t>
         </is>
       </c>
     </row>
@@ -2975,14 +2975,14 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.8586956521739131</v>
+        <v>0.8905583972719523</v>
       </c>
       <c r="E91" t="n">
-        <v>0.03804347826086951</v>
+        <v>0.013000852514919</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[0.8478260869565217, 0.8695652173913043, 0.8695652173913043, 0.8695652173913043, 0.8695652173913043, 0.8260869565217391, 0.8478260869565217, 0.8695652173913043, 0.8260869565217391, 0.8260869565217391]</t>
+          <t>[0.8970588235294118, 0.8840579710144928, 0.8840579710144928, 0.8840579710144928, 0.8695652173913043, 0.9117647058823529, 0.8840579710144928, 0.8970588235294118, 0.8970588235294118, 0.8970588235294118]</t>
         </is>
       </c>
     </row>
@@ -3003,14 +3003,14 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.9165695415695416</v>
+        <v>0.8741258741258741</v>
       </c>
       <c r="E92" t="n">
-        <v>0.01888368983957223</v>
+        <v>0.02977022977022981</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>[0.9020979020979021, 0.9242424242424243, 0.9292929292929293, 0.9557109557109557, 0.9324009324009324, 0.9217171717171717, 0.9114219114219114, 0.9015151515151515, 0.9093137254901961, 0.9090909090909092]</t>
+          <t>[0.8601398601398601, 0.8713286713286713, 0.8769230769230768, 0.8467532467532468, 0.8857142857142857, 0.8545454545454546, 0.9118881118881119, 0.8597402597402598, 0.8909090909090909, 0.9062937062937063]</t>
         </is>
       </c>
     </row>
@@ -3031,14 +3031,14 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0.8549394332684404</v>
+        <v>0.8805537627047925</v>
       </c>
       <c r="E93" t="n">
-        <v>0.03281391953277091</v>
+        <v>0.01957607544172701</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>[0.8497339390006488, 0.8695652173913043, 0.8697115384615384, 0.8695652173913043, 0.8695652173913043, 0.833695652173913, 0.8459182349123945, 0.860144927536232, 0.8206662902315077, 0.8295807453416149]</t>
+          <t>[0.8846773194599282, 0.8764302059496567, 0.8712461950842759, 0.8764302059496567, 0.8677373025199112, 0.9073226544622426, 0.8647998034880864, 0.8954636989931107, 0.8938104399127871, 0.8870417732310315]</t>
         </is>
       </c>
     </row>
@@ -3059,14 +3059,14 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.7497094184737205</v>
+        <v>0.7905039278036989</v>
       </c>
       <c r="E94" t="n">
-        <v>0.03457514118121319</v>
+        <v>0.02821161422803498</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>[0.725281803542673, 0.7188735177865612, 0.7047839716505383, 0.7690396023729357, 0.7494824016563146, 0.7517241379310345, 0.7748677248677249, 0.7913869276188117, 0.7446969696969697, 0.7499364352911264]</t>
+          <t>[0.7571759987417427, 0.7617647058823529, 0.7729468599033815, 0.8047870004391744, 0.7803652353389868, 0.7929414328660527, 0.7976912706437479, 0.807918552036199, 0.8074596335465901, 0.7880664227413453]</t>
         </is>
       </c>
     </row>
@@ -3087,14 +3087,14 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>0.7473429951690821</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="E95" t="n">
-        <v>0.03816425120772948</v>
+        <v>0.0282395566922421</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[0.717391304347826, 0.7111111111111111, 0.717391304347826, 0.7555555555555555, 0.7608695652173914, 0.7555555555555555, 0.7777777777777778, 0.7777777777777778, 0.7333333333333333, 0.7391304347826086]</t>
+          <t>[0.75, 0.7536231884057971, 0.7681159420289855, 0.7971014492753623, 0.782608695652174, 0.782608695652174, 0.7681159420289855, 0.8088235294117647, 0.8115942028985508, 0.7941176470588235]</t>
         </is>
       </c>
     </row>
@@ -3115,14 +3115,14 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>0.8940147282710211</v>
+        <v>0.9172683355292051</v>
       </c>
       <c r="E96" t="n">
-        <v>0.0306975701500537</v>
+        <v>0.008686239688563191</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>[0.8673883324913073, 0.9066339066339067, 0.8400472525186484, 0.8826722228256755, 0.9016241195875062, 0.872021112021112, 0.9354691054691054, 0.888039858039858, 0.914961324961325, 0.8999895985021843]</t>
+          <t>[0.9124186606460766, 0.9241106719367589, 0.9198770311813791, 0.9016731692677071, 0.9212334933973589, 0.9146596398770311, 0.9128062588671833, 0.9251559068950375, 0.921106719367589, 0.9115063680281073]</t>
         </is>
       </c>
     </row>
@@ -3143,14 +3143,14 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0.7408184443933236</v>
+        <v>0.7809651102077468</v>
       </c>
       <c r="E97" t="n">
-        <v>0.03643093107653927</v>
+        <v>0.03821413607573332</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[0.7169593444473906, 0.7037134927976743, 0.705774097078445, 0.7588759453590493, 0.75181061760225, 0.7443621399176954, 0.771069182389937, 0.7831045751633986, 0.7372747488689517, 0.7318366960310694]</t>
+          <t>[0.7519942611190817, 0.7528643849488618, 0.7617889357019793, 0.7977870381962454, 0.7805414109761936, 0.7813888094393002, 0.7562310373537671, 0.8053452685421995, 0.8086278498177812, 0.7899774774774775]</t>
         </is>
       </c>
     </row>

</xml_diff>